<commit_message>
Update RMI_pH Water Sample Log.xlsx
</commit_message>
<xml_diff>
--- a/pH_glider/water_sampling/sample_logs/RMI_pH Water Sample Log.xlsx
+++ b/pH_glider/water_sampling/sample_logs/RMI_pH Water Sample Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garzio/Documents/repo/rucool/dataset_archiving/pH_glider/water_sampling/sample_logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B92179A-8500-0141-AE86-88FE15AA4549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3965E6F-773B-9444-8106-8D498A230E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="1100" windowWidth="28460" windowHeight="18840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2025,66 +2025,6 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2097,8 +2037,68 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -3387,11 +3387,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V250"/>
+  <dimension ref="A1:U245"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="L1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q248" sqref="Q248:S250"/>
+      <selection pane="bottomLeft" activeCell="W252" sqref="W252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3482,7 +3482,7 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="90" t="s">
+      <c r="A2" s="92" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="6">
@@ -3497,7 +3497,7 @@
       <c r="E2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="90" t="s">
+      <c r="F2" s="92" t="s">
         <v>98</v>
       </c>
       <c r="G2" s="8" t="s">
@@ -3541,7 +3541,7 @@
       <c r="U2" s="22"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" s="91"/>
+      <c r="A3" s="93"/>
       <c r="B3" s="6">
         <v>45036</v>
       </c>
@@ -3554,7 +3554,7 @@
       <c r="E3" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="91"/>
+      <c r="F3" s="93"/>
       <c r="G3" s="8" t="s">
         <v>18</v>
       </c>
@@ -3594,7 +3594,7 @@
       <c r="U3" s="22"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A4" s="91"/>
+      <c r="A4" s="93"/>
       <c r="B4" s="6">
         <v>45036</v>
       </c>
@@ -3607,7 +3607,7 @@
       <c r="E4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="91"/>
+      <c r="F4" s="93"/>
       <c r="G4" s="8" t="s">
         <v>19</v>
       </c>
@@ -3649,7 +3649,7 @@
       <c r="U4" s="22"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A5" s="91"/>
+      <c r="A5" s="93"/>
       <c r="B5" s="6">
         <v>45036</v>
       </c>
@@ -3662,7 +3662,7 @@
       <c r="E5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="91"/>
+      <c r="F5" s="93"/>
       <c r="G5" s="8" t="s">
         <v>20</v>
       </c>
@@ -3702,7 +3702,7 @@
       <c r="U5" s="22"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A6" s="91"/>
+      <c r="A6" s="93"/>
       <c r="B6" s="6">
         <v>45036</v>
       </c>
@@ -3715,7 +3715,7 @@
       <c r="E6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="91"/>
+      <c r="F6" s="93"/>
       <c r="G6" s="8" t="s">
         <v>21</v>
       </c>
@@ -3757,7 +3757,7 @@
       <c r="U6" s="22"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A7" s="91"/>
+      <c r="A7" s="93"/>
       <c r="B7" s="6">
         <v>45036</v>
       </c>
@@ -3770,7 +3770,7 @@
       <c r="E7" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="91"/>
+      <c r="F7" s="93"/>
       <c r="G7" s="8" t="s">
         <v>22</v>
       </c>
@@ -3810,7 +3810,7 @@
       <c r="U7" s="22"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A8" s="91"/>
+      <c r="A8" s="93"/>
       <c r="B8" s="6">
         <v>45036</v>
       </c>
@@ -3823,7 +3823,7 @@
       <c r="E8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="91"/>
+      <c r="F8" s="93"/>
       <c r="G8" s="8" t="s">
         <v>23</v>
       </c>
@@ -3865,7 +3865,7 @@
       <c r="U8" s="22"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A9" s="91"/>
+      <c r="A9" s="93"/>
       <c r="B9" s="6">
         <v>45036</v>
       </c>
@@ -3878,7 +3878,7 @@
       <c r="E9" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="91"/>
+      <c r="F9" s="93"/>
       <c r="G9" s="8" t="s">
         <v>24</v>
       </c>
@@ -3918,7 +3918,7 @@
       <c r="U9" s="22"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A10" s="91"/>
+      <c r="A10" s="93"/>
       <c r="B10" s="6">
         <v>45036</v>
       </c>
@@ -3931,7 +3931,7 @@
       <c r="E10" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="91"/>
+      <c r="F10" s="93"/>
       <c r="G10" s="8" t="s">
         <v>25</v>
       </c>
@@ -3973,7 +3973,7 @@
       <c r="U10" s="22"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A11" s="91"/>
+      <c r="A11" s="93"/>
       <c r="B11" s="6">
         <v>45036</v>
       </c>
@@ -3986,7 +3986,7 @@
       <c r="E11" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="91"/>
+      <c r="F11" s="93"/>
       <c r="G11" s="8" t="s">
         <v>26</v>
       </c>
@@ -4026,7 +4026,7 @@
       <c r="U11" s="22"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A12" s="91"/>
+      <c r="A12" s="93"/>
       <c r="B12" s="6">
         <v>45036</v>
       </c>
@@ -4039,7 +4039,7 @@
       <c r="E12" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="91"/>
+      <c r="F12" s="93"/>
       <c r="G12" s="8" t="s">
         <v>27</v>
       </c>
@@ -4081,7 +4081,7 @@
       <c r="U12" s="22"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A13" s="92"/>
+      <c r="A13" s="94"/>
       <c r="B13" s="6">
         <v>45036</v>
       </c>
@@ -4094,7 +4094,7 @@
       <c r="E13" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="92"/>
+      <c r="F13" s="94"/>
       <c r="G13" s="8" t="s">
         <v>28</v>
       </c>
@@ -4134,7 +4134,7 @@
       <c r="U13" s="22"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A14" s="93" t="s">
+      <c r="A14" s="98" t="s">
         <v>36</v>
       </c>
       <c r="B14" s="3">
@@ -4149,7 +4149,7 @@
       <c r="E14" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="F14" s="93" t="s">
+      <c r="F14" s="98" t="s">
         <v>99</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -4193,7 +4193,7 @@
       <c r="U14" s="17"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A15" s="94"/>
+      <c r="A15" s="99"/>
       <c r="B15" s="3">
         <v>45058</v>
       </c>
@@ -4206,7 +4206,7 @@
       <c r="E15" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="F15" s="94"/>
+      <c r="F15" s="99"/>
       <c r="G15" s="2" t="s">
         <v>38</v>
       </c>
@@ -4246,7 +4246,7 @@
       <c r="U15" s="17"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A16" s="94"/>
+      <c r="A16" s="99"/>
       <c r="B16" s="3">
         <v>45058</v>
       </c>
@@ -4259,7 +4259,7 @@
       <c r="E16" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="F16" s="94"/>
+      <c r="F16" s="99"/>
       <c r="G16" s="2" t="s">
         <v>39</v>
       </c>
@@ -4301,7 +4301,7 @@
       <c r="U16" s="17"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A17" s="94"/>
+      <c r="A17" s="99"/>
       <c r="B17" s="3">
         <v>45058</v>
       </c>
@@ -4314,7 +4314,7 @@
       <c r="E17" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="F17" s="94"/>
+      <c r="F17" s="99"/>
       <c r="G17" s="2" t="s">
         <v>40</v>
       </c>
@@ -4354,7 +4354,7 @@
       <c r="U17" s="17"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A18" s="94"/>
+      <c r="A18" s="99"/>
       <c r="B18" s="3">
         <v>45058</v>
       </c>
@@ -4367,7 +4367,7 @@
       <c r="E18" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="F18" s="94"/>
+      <c r="F18" s="99"/>
       <c r="G18" s="2" t="s">
         <v>41</v>
       </c>
@@ -4409,7 +4409,7 @@
       <c r="U18" s="17"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A19" s="94"/>
+      <c r="A19" s="99"/>
       <c r="B19" s="3">
         <v>45058</v>
       </c>
@@ -4422,7 +4422,7 @@
       <c r="E19" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="F19" s="94"/>
+      <c r="F19" s="99"/>
       <c r="G19" s="2" t="s">
         <v>42</v>
       </c>
@@ -4462,7 +4462,7 @@
       <c r="U19" s="17"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A20" s="94"/>
+      <c r="A20" s="99"/>
       <c r="B20" s="3">
         <v>45058</v>
       </c>
@@ -4475,7 +4475,7 @@
       <c r="E20" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="F20" s="94"/>
+      <c r="F20" s="99"/>
       <c r="G20" s="2" t="s">
         <v>43</v>
       </c>
@@ -4517,7 +4517,7 @@
       <c r="U20" s="17"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A21" s="94"/>
+      <c r="A21" s="99"/>
       <c r="B21" s="3">
         <v>45058</v>
       </c>
@@ -4530,7 +4530,7 @@
       <c r="E21" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="F21" s="94"/>
+      <c r="F21" s="99"/>
       <c r="G21" s="2" t="s">
         <v>44</v>
       </c>
@@ -4570,7 +4570,7 @@
       <c r="U21" s="17"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A22" s="94"/>
+      <c r="A22" s="99"/>
       <c r="B22" s="3">
         <v>45058</v>
       </c>
@@ -4583,7 +4583,7 @@
       <c r="E22" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="F22" s="94"/>
+      <c r="F22" s="99"/>
       <c r="G22" s="2" t="s">
         <v>45</v>
       </c>
@@ -4625,7 +4625,7 @@
       <c r="U22" s="17"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A23" s="94"/>
+      <c r="A23" s="99"/>
       <c r="B23" s="3">
         <v>45058</v>
       </c>
@@ -4638,7 +4638,7 @@
       <c r="E23" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="F23" s="94"/>
+      <c r="F23" s="99"/>
       <c r="G23" s="2" t="s">
         <v>46</v>
       </c>
@@ -4678,7 +4678,7 @@
       <c r="U23" s="17"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A24" s="94"/>
+      <c r="A24" s="99"/>
       <c r="B24" s="3">
         <v>45058</v>
       </c>
@@ -4691,7 +4691,7 @@
       <c r="E24" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="F24" s="94"/>
+      <c r="F24" s="99"/>
       <c r="G24" s="2" t="s">
         <v>47</v>
       </c>
@@ -4733,7 +4733,7 @@
       <c r="U24" s="17"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A25" s="95"/>
+      <c r="A25" s="100"/>
       <c r="B25" s="3">
         <v>45058</v>
       </c>
@@ -4746,7 +4746,7 @@
       <c r="E25" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="F25" s="95"/>
+      <c r="F25" s="100"/>
       <c r="G25" s="2" t="s">
         <v>48</v>
       </c>
@@ -4786,7 +4786,7 @@
       <c r="U25" s="17"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A26" s="90" t="s">
+      <c r="A26" s="92" t="s">
         <v>49</v>
       </c>
       <c r="B26" s="6">
@@ -4801,7 +4801,7 @@
       <c r="E26" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="F26" s="90" t="s">
+      <c r="F26" s="92" t="s">
         <v>100</v>
       </c>
       <c r="G26" s="8" t="s">
@@ -4845,7 +4845,7 @@
       <c r="U26" s="22"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A27" s="91"/>
+      <c r="A27" s="93"/>
       <c r="B27" s="6">
         <v>45155</v>
       </c>
@@ -4858,7 +4858,7 @@
       <c r="E27" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="F27" s="91"/>
+      <c r="F27" s="93"/>
       <c r="G27" s="8" t="s">
         <v>52</v>
       </c>
@@ -4898,7 +4898,7 @@
       <c r="U27" s="22"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A28" s="91"/>
+      <c r="A28" s="93"/>
       <c r="B28" s="6">
         <v>45155</v>
       </c>
@@ -4911,7 +4911,7 @@
       <c r="E28" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="F28" s="91"/>
+      <c r="F28" s="93"/>
       <c r="G28" s="8" t="s">
         <v>53</v>
       </c>
@@ -4955,7 +4955,7 @@
       <c r="U28" s="22"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A29" s="91"/>
+      <c r="A29" s="93"/>
       <c r="B29" s="6">
         <v>45155</v>
       </c>
@@ -4968,7 +4968,7 @@
       <c r="E29" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="F29" s="91"/>
+      <c r="F29" s="93"/>
       <c r="G29" s="8" t="s">
         <v>54</v>
       </c>
@@ -5010,7 +5010,7 @@
       <c r="U29" s="22"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A30" s="91"/>
+      <c r="A30" s="93"/>
       <c r="B30" s="6">
         <v>45155</v>
       </c>
@@ -5023,7 +5023,7 @@
       <c r="E30" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="F30" s="91"/>
+      <c r="F30" s="93"/>
       <c r="G30" s="8" t="s">
         <v>55</v>
       </c>
@@ -5065,7 +5065,7 @@
       <c r="U30" s="22"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A31" s="91"/>
+      <c r="A31" s="93"/>
       <c r="B31" s="6">
         <v>45155</v>
       </c>
@@ -5078,7 +5078,7 @@
       <c r="E31" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="91"/>
+      <c r="F31" s="93"/>
       <c r="G31" s="8" t="s">
         <v>56</v>
       </c>
@@ -5118,7 +5118,7 @@
       <c r="U31" s="22"/>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A32" s="91"/>
+      <c r="A32" s="93"/>
       <c r="B32" s="6">
         <v>45155</v>
       </c>
@@ -5131,7 +5131,7 @@
       <c r="E32" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="F32" s="91"/>
+      <c r="F32" s="93"/>
       <c r="G32" s="8" t="s">
         <v>57</v>
       </c>
@@ -5173,7 +5173,7 @@
       <c r="U32" s="22"/>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A33" s="91"/>
+      <c r="A33" s="93"/>
       <c r="B33" s="6">
         <v>45155</v>
       </c>
@@ -5186,7 +5186,7 @@
       <c r="E33" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="F33" s="91"/>
+      <c r="F33" s="93"/>
       <c r="G33" s="8" t="s">
         <v>58</v>
       </c>
@@ -5226,7 +5226,7 @@
       <c r="U33" s="22"/>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A34" s="91"/>
+      <c r="A34" s="93"/>
       <c r="B34" s="6">
         <v>45155</v>
       </c>
@@ -5239,7 +5239,7 @@
       <c r="E34" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="F34" s="91"/>
+      <c r="F34" s="93"/>
       <c r="G34" s="8" t="s">
         <v>59</v>
       </c>
@@ -5281,7 +5281,7 @@
       <c r="U34" s="22"/>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A35" s="91"/>
+      <c r="A35" s="93"/>
       <c r="B35" s="6">
         <v>45155</v>
       </c>
@@ -5294,7 +5294,7 @@
       <c r="E35" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="F35" s="91"/>
+      <c r="F35" s="93"/>
       <c r="G35" s="8" t="s">
         <v>60</v>
       </c>
@@ -5334,7 +5334,7 @@
       <c r="U35" s="22"/>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A36" s="91"/>
+      <c r="A36" s="93"/>
       <c r="B36" s="6">
         <v>45155</v>
       </c>
@@ -5347,7 +5347,7 @@
       <c r="E36" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="F36" s="91"/>
+      <c r="F36" s="93"/>
       <c r="G36" s="8" t="s">
         <v>50</v>
       </c>
@@ -5389,7 +5389,7 @@
       <c r="U36" s="22"/>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A37" s="92"/>
+      <c r="A37" s="94"/>
       <c r="B37" s="6">
         <v>45155</v>
       </c>
@@ -5402,7 +5402,7 @@
       <c r="E37" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="F37" s="92"/>
+      <c r="F37" s="94"/>
       <c r="G37" s="8" t="s">
         <v>61</v>
       </c>
@@ -5442,7 +5442,7 @@
       <c r="U37" s="22"/>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A38" s="93" t="s">
+      <c r="A38" s="98" t="s">
         <v>67</v>
       </c>
       <c r="B38" s="3">
@@ -5457,7 +5457,7 @@
       <c r="E38" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F38" s="93" t="s">
+      <c r="F38" s="98" t="s">
         <v>78</v>
       </c>
       <c r="G38" s="2" t="s">
@@ -5503,7 +5503,7 @@
       <c r="U38" s="17"/>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A39" s="94"/>
+      <c r="A39" s="99"/>
       <c r="B39" s="3">
         <v>45189</v>
       </c>
@@ -5516,7 +5516,7 @@
       <c r="E39" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F39" s="103"/>
+      <c r="F39" s="109"/>
       <c r="G39" s="2" t="s">
         <v>69</v>
       </c>
@@ -5558,7 +5558,7 @@
       <c r="U39" s="17"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A40" s="94"/>
+      <c r="A40" s="99"/>
       <c r="B40" s="3">
         <v>45189</v>
       </c>
@@ -5571,7 +5571,7 @@
       <c r="E40" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F40" s="103"/>
+      <c r="F40" s="109"/>
       <c r="G40" s="2" t="s">
         <v>70</v>
       </c>
@@ -5615,7 +5615,7 @@
       <c r="U40" s="17"/>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A41" s="94"/>
+      <c r="A41" s="99"/>
       <c r="B41" s="3">
         <v>45189</v>
       </c>
@@ -5628,7 +5628,7 @@
       <c r="E41" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F41" s="103"/>
+      <c r="F41" s="109"/>
       <c r="G41" s="2" t="s">
         <v>71</v>
       </c>
@@ -5670,7 +5670,7 @@
       <c r="U41" s="17"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A42" s="94"/>
+      <c r="A42" s="99"/>
       <c r="B42" s="3">
         <v>45189</v>
       </c>
@@ -5683,7 +5683,7 @@
       <c r="E42" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F42" s="103"/>
+      <c r="F42" s="109"/>
       <c r="G42" s="2" t="s">
         <v>72</v>
       </c>
@@ -5727,7 +5727,7 @@
       <c r="U42" s="17"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A43" s="94"/>
+      <c r="A43" s="99"/>
       <c r="B43" s="3">
         <v>45189</v>
       </c>
@@ -5740,7 +5740,7 @@
       <c r="E43" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F43" s="103"/>
+      <c r="F43" s="109"/>
       <c r="G43" s="2" t="s">
         <v>73</v>
       </c>
@@ -5782,7 +5782,7 @@
       <c r="U43" s="17"/>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A44" s="94"/>
+      <c r="A44" s="99"/>
       <c r="B44" s="3">
         <v>45189</v>
       </c>
@@ -5795,7 +5795,7 @@
       <c r="E44" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F44" s="103"/>
+      <c r="F44" s="109"/>
       <c r="G44" s="2" t="s">
         <v>74</v>
       </c>
@@ -5839,7 +5839,7 @@
       <c r="U44" s="17"/>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A45" s="94"/>
+      <c r="A45" s="99"/>
       <c r="B45" s="3">
         <v>45189</v>
       </c>
@@ -5852,7 +5852,7 @@
       <c r="E45" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F45" s="104"/>
+      <c r="F45" s="110"/>
       <c r="G45" s="2" t="s">
         <v>75</v>
       </c>
@@ -5894,7 +5894,7 @@
       <c r="U45" s="17"/>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A46" s="90" t="s">
+      <c r="A46" s="92" t="s">
         <v>93</v>
       </c>
       <c r="B46" s="6">
@@ -5909,7 +5909,7 @@
       <c r="E46" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="F46" s="90" t="s">
+      <c r="F46" s="92" t="s">
         <v>118</v>
       </c>
       <c r="G46" s="8" t="s">
@@ -5955,7 +5955,7 @@
       <c r="U46" s="24"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A47" s="91"/>
+      <c r="A47" s="93"/>
       <c r="B47" s="6">
         <v>45189</v>
       </c>
@@ -5968,7 +5968,7 @@
       <c r="E47" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="F47" s="91"/>
+      <c r="F47" s="93"/>
       <c r="G47" s="8" t="s">
         <v>82</v>
       </c>
@@ -6012,7 +6012,7 @@
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A48" s="91"/>
+      <c r="A48" s="93"/>
       <c r="B48" s="6">
         <v>45189</v>
       </c>
@@ -6025,7 +6025,7 @@
       <c r="E48" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="F48" s="91"/>
+      <c r="F48" s="93"/>
       <c r="G48" s="8" t="s">
         <v>83</v>
       </c>
@@ -6069,7 +6069,7 @@
       <c r="U48" s="24"/>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A49" s="91"/>
+      <c r="A49" s="93"/>
       <c r="B49" s="6">
         <v>45189</v>
       </c>
@@ -6082,7 +6082,7 @@
       <c r="E49" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="F49" s="91"/>
+      <c r="F49" s="93"/>
       <c r="G49" s="8" t="s">
         <v>84</v>
       </c>
@@ -6126,7 +6126,7 @@
       </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A50" s="91"/>
+      <c r="A50" s="93"/>
       <c r="B50" s="6">
         <v>45189</v>
       </c>
@@ -6139,7 +6139,7 @@
       <c r="E50" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="F50" s="91"/>
+      <c r="F50" s="93"/>
       <c r="G50" s="8" t="s">
         <v>85</v>
       </c>
@@ -6183,7 +6183,7 @@
       <c r="U50" s="22"/>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A51" s="91"/>
+      <c r="A51" s="93"/>
       <c r="B51" s="6">
         <v>45189</v>
       </c>
@@ -6196,7 +6196,7 @@
       <c r="E51" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="F51" s="91"/>
+      <c r="F51" s="93"/>
       <c r="G51" s="8" t="s">
         <v>86</v>
       </c>
@@ -6238,7 +6238,7 @@
       <c r="U51" s="22"/>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A52" s="91"/>
+      <c r="A52" s="93"/>
       <c r="B52" s="6">
         <v>45189</v>
       </c>
@@ -6251,7 +6251,7 @@
       <c r="E52" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="F52" s="91"/>
+      <c r="F52" s="93"/>
       <c r="G52" s="8" t="s">
         <v>87</v>
       </c>
@@ -6295,7 +6295,7 @@
       <c r="U52" s="22"/>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A53" s="91"/>
+      <c r="A53" s="93"/>
       <c r="B53" s="6">
         <v>45189</v>
       </c>
@@ -6308,7 +6308,7 @@
       <c r="E53" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="F53" s="91"/>
+      <c r="F53" s="93"/>
       <c r="G53" s="8" t="s">
         <v>88</v>
       </c>
@@ -6352,7 +6352,7 @@
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A54" s="91"/>
+      <c r="A54" s="93"/>
       <c r="B54" s="6">
         <v>45189</v>
       </c>
@@ -6365,7 +6365,7 @@
       <c r="E54" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="F54" s="91"/>
+      <c r="F54" s="93"/>
       <c r="G54" s="8" t="s">
         <v>89</v>
       </c>
@@ -6409,7 +6409,7 @@
       <c r="U54" s="22"/>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A55" s="91"/>
+      <c r="A55" s="93"/>
       <c r="B55" s="6">
         <v>45189</v>
       </c>
@@ -6422,7 +6422,7 @@
       <c r="E55" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="F55" s="91"/>
+      <c r="F55" s="93"/>
       <c r="G55" s="8" t="s">
         <v>90</v>
       </c>
@@ -6464,7 +6464,7 @@
       <c r="U55" s="22"/>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A56" s="91"/>
+      <c r="A56" s="93"/>
       <c r="B56" s="6">
         <v>45189</v>
       </c>
@@ -6477,7 +6477,7 @@
       <c r="E56" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="F56" s="91"/>
+      <c r="F56" s="93"/>
       <c r="G56" s="8" t="s">
         <v>91</v>
       </c>
@@ -6521,7 +6521,7 @@
       <c r="U56" s="22"/>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A57" s="92"/>
+      <c r="A57" s="94"/>
       <c r="B57" s="6">
         <v>45189</v>
       </c>
@@ -6534,7 +6534,7 @@
       <c r="E57" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="F57" s="92"/>
+      <c r="F57" s="94"/>
       <c r="G57" s="8" t="s">
         <v>92</v>
       </c>
@@ -6576,7 +6576,7 @@
       <c r="U57" s="22"/>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A58" s="93" t="s">
+      <c r="A58" s="98" t="s">
         <v>104</v>
       </c>
       <c r="B58" s="3">
@@ -6591,7 +6591,7 @@
       <c r="E58" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F58" s="93" t="s">
+      <c r="F58" s="98" t="s">
         <v>143</v>
       </c>
       <c r="G58" s="2" t="s">
@@ -6637,7 +6637,7 @@
       <c r="U58" s="17"/>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A59" s="94"/>
+      <c r="A59" s="99"/>
       <c r="B59" s="3">
         <v>45217</v>
       </c>
@@ -6650,7 +6650,7 @@
       <c r="E59" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F59" s="103"/>
+      <c r="F59" s="109"/>
       <c r="G59" s="2" t="s">
         <v>106</v>
       </c>
@@ -6692,7 +6692,7 @@
       <c r="U59" s="17"/>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A60" s="94"/>
+      <c r="A60" s="99"/>
       <c r="B60" s="3">
         <v>45217</v>
       </c>
@@ -6705,7 +6705,7 @@
       <c r="E60" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F60" s="103"/>
+      <c r="F60" s="109"/>
       <c r="G60" s="2" t="s">
         <v>107</v>
       </c>
@@ -6749,7 +6749,7 @@
       <c r="U60" s="17"/>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A61" s="94"/>
+      <c r="A61" s="99"/>
       <c r="B61" s="3">
         <v>45217</v>
       </c>
@@ -6762,7 +6762,7 @@
       <c r="E61" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F61" s="103"/>
+      <c r="F61" s="109"/>
       <c r="G61" s="2" t="s">
         <v>108</v>
       </c>
@@ -6804,7 +6804,7 @@
       <c r="U61" s="17"/>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A62" s="94"/>
+      <c r="A62" s="99"/>
       <c r="B62" s="3">
         <v>45217</v>
       </c>
@@ -6817,7 +6817,7 @@
       <c r="E62" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F62" s="103"/>
+      <c r="F62" s="109"/>
       <c r="G62" s="2" t="s">
         <v>109</v>
       </c>
@@ -6861,7 +6861,7 @@
       <c r="U62" s="17"/>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A63" s="94"/>
+      <c r="A63" s="99"/>
       <c r="B63" s="3">
         <v>45217</v>
       </c>
@@ -6874,7 +6874,7 @@
       <c r="E63" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F63" s="103"/>
+      <c r="F63" s="109"/>
       <c r="G63" s="2" t="s">
         <v>110</v>
       </c>
@@ -6916,7 +6916,7 @@
       <c r="U63" s="17"/>
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A64" s="94"/>
+      <c r="A64" s="99"/>
       <c r="B64" s="3">
         <v>45217</v>
       </c>
@@ -6929,7 +6929,7 @@
       <c r="E64" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F64" s="103"/>
+      <c r="F64" s="109"/>
       <c r="G64" s="2" t="s">
         <v>111</v>
       </c>
@@ -6973,7 +6973,7 @@
       <c r="U64" s="17"/>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A65" s="94"/>
+      <c r="A65" s="99"/>
       <c r="B65" s="3">
         <v>45217</v>
       </c>
@@ -6986,7 +6986,7 @@
       <c r="E65" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F65" s="104"/>
+      <c r="F65" s="110"/>
       <c r="G65" s="2" t="s">
         <v>112</v>
       </c>
@@ -7028,7 +7028,7 @@
       <c r="U65" s="17"/>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A66" s="90" t="s">
+      <c r="A66" s="92" t="s">
         <v>119</v>
       </c>
       <c r="B66" s="6">
@@ -7043,7 +7043,7 @@
       <c r="E66" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="F66" s="90" t="s">
+      <c r="F66" s="92" t="s">
         <v>142</v>
       </c>
       <c r="G66" s="8" t="s">
@@ -7089,7 +7089,7 @@
       <c r="U66" s="22"/>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A67" s="91"/>
+      <c r="A67" s="93"/>
       <c r="B67" s="6">
         <v>45218</v>
       </c>
@@ -7102,7 +7102,7 @@
       <c r="E67" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="F67" s="91"/>
+      <c r="F67" s="93"/>
       <c r="G67" s="8" t="s">
         <v>121</v>
       </c>
@@ -7144,7 +7144,7 @@
       <c r="U67" s="22"/>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A68" s="91"/>
+      <c r="A68" s="93"/>
       <c r="B68" s="6">
         <v>45218</v>
       </c>
@@ -7157,7 +7157,7 @@
       <c r="E68" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="F68" s="91"/>
+      <c r="F68" s="93"/>
       <c r="G68" s="8" t="s">
         <v>122</v>
       </c>
@@ -7201,7 +7201,7 @@
       <c r="U68" s="22"/>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A69" s="91"/>
+      <c r="A69" s="93"/>
       <c r="B69" s="6">
         <v>45218</v>
       </c>
@@ -7214,7 +7214,7 @@
       <c r="E69" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="F69" s="91"/>
+      <c r="F69" s="93"/>
       <c r="G69" s="8" t="s">
         <v>123</v>
       </c>
@@ -7256,7 +7256,7 @@
       <c r="U69" s="22"/>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A70" s="91"/>
+      <c r="A70" s="93"/>
       <c r="B70" s="6">
         <v>45218</v>
       </c>
@@ -7269,7 +7269,7 @@
       <c r="E70" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="F70" s="91"/>
+      <c r="F70" s="93"/>
       <c r="G70" s="8" t="s">
         <v>124</v>
       </c>
@@ -7313,7 +7313,7 @@
       <c r="U70" s="22"/>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A71" s="91"/>
+      <c r="A71" s="93"/>
       <c r="B71" s="6">
         <v>45218</v>
       </c>
@@ -7326,7 +7326,7 @@
       <c r="E71" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="F71" s="91"/>
+      <c r="F71" s="93"/>
       <c r="G71" s="8" t="s">
         <v>125</v>
       </c>
@@ -7368,7 +7368,7 @@
       <c r="U71" s="22"/>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A72" s="91"/>
+      <c r="A72" s="93"/>
       <c r="B72" s="6">
         <v>45218</v>
       </c>
@@ -7381,7 +7381,7 @@
       <c r="E72" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="F72" s="91"/>
+      <c r="F72" s="93"/>
       <c r="G72" s="8" t="s">
         <v>126</v>
       </c>
@@ -7425,7 +7425,7 @@
       <c r="U72" s="22"/>
     </row>
     <row r="73" spans="1:21" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="91"/>
+      <c r="A73" s="93"/>
       <c r="B73" s="6">
         <v>45218</v>
       </c>
@@ -7438,7 +7438,7 @@
       <c r="E73" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="F73" s="91"/>
+      <c r="F73" s="93"/>
       <c r="G73" s="8" t="s">
         <v>127</v>
       </c>
@@ -7480,7 +7480,7 @@
       <c r="U73" s="22"/>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A74" s="93" t="s">
+      <c r="A74" s="98" t="s">
         <v>132</v>
       </c>
       <c r="B74" s="3">
@@ -7495,7 +7495,7 @@
       <c r="E74" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="F74" s="93" t="s">
+      <c r="F74" s="98" t="s">
         <v>141</v>
       </c>
       <c r="G74" s="2" t="s">
@@ -7543,7 +7543,7 @@
       </c>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A75" s="94"/>
+      <c r="A75" s="99"/>
       <c r="B75" s="3">
         <v>45233</v>
       </c>
@@ -7556,7 +7556,7 @@
       <c r="E75" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="F75" s="103"/>
+      <c r="F75" s="109"/>
       <c r="G75" s="2" t="s">
         <v>138</v>
       </c>
@@ -7598,7 +7598,7 @@
       <c r="U75" s="2"/>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A76" s="94"/>
+      <c r="A76" s="99"/>
       <c r="B76" s="3">
         <v>45233</v>
       </c>
@@ -7611,7 +7611,7 @@
       <c r="E76" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F76" s="103"/>
+      <c r="F76" s="109"/>
       <c r="G76" s="2" t="s">
         <v>139</v>
       </c>
@@ -7655,7 +7655,7 @@
       <c r="U76" s="2"/>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A77" s="94"/>
+      <c r="A77" s="99"/>
       <c r="B77" s="3">
         <v>45233</v>
       </c>
@@ -7668,7 +7668,7 @@
       <c r="E77" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F77" s="103"/>
+      <c r="F77" s="109"/>
       <c r="G77" s="2" t="s">
         <v>140</v>
       </c>
@@ -7710,7 +7710,7 @@
       <c r="U77" s="2"/>
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A78" s="90" t="s">
+      <c r="A78" s="92" t="s">
         <v>144</v>
       </c>
       <c r="B78" s="6">
@@ -7725,7 +7725,7 @@
       <c r="E78" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="F78" s="90" t="s">
+      <c r="F78" s="92" t="s">
         <v>156</v>
       </c>
       <c r="G78" s="8" t="s">
@@ -7771,7 +7771,7 @@
       <c r="U78" s="8"/>
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A79" s="91"/>
+      <c r="A79" s="93"/>
       <c r="B79" s="6">
         <v>45265</v>
       </c>
@@ -7784,7 +7784,7 @@
       <c r="E79" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="F79" s="91"/>
+      <c r="F79" s="93"/>
       <c r="G79" s="8" t="s">
         <v>149</v>
       </c>
@@ -7826,7 +7826,7 @@
       <c r="U79" s="8"/>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A80" s="91"/>
+      <c r="A80" s="93"/>
       <c r="B80" s="6">
         <v>45265</v>
       </c>
@@ -7839,7 +7839,7 @@
       <c r="E80" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="F80" s="91"/>
+      <c r="F80" s="93"/>
       <c r="G80" s="8" t="s">
         <v>150</v>
       </c>
@@ -7883,7 +7883,7 @@
       <c r="U80" s="8"/>
     </row>
     <row r="81" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A81" s="91"/>
+      <c r="A81" s="93"/>
       <c r="B81" s="6">
         <v>45265</v>
       </c>
@@ -7896,7 +7896,7 @@
       <c r="E81" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="F81" s="91"/>
+      <c r="F81" s="93"/>
       <c r="G81" s="8" t="s">
         <v>151</v>
       </c>
@@ -7938,7 +7938,7 @@
       <c r="U81" s="8"/>
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A82" s="91"/>
+      <c r="A82" s="93"/>
       <c r="B82" s="6">
         <v>45265</v>
       </c>
@@ -7951,7 +7951,7 @@
       <c r="E82" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="F82" s="91"/>
+      <c r="F82" s="93"/>
       <c r="G82" s="8" t="s">
         <v>152</v>
       </c>
@@ -7995,7 +7995,7 @@
       <c r="U82" s="8"/>
     </row>
     <row r="83" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A83" s="91"/>
+      <c r="A83" s="93"/>
       <c r="B83" s="6">
         <v>45265</v>
       </c>
@@ -8008,7 +8008,7 @@
       <c r="E83" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="F83" s="91"/>
+      <c r="F83" s="93"/>
       <c r="G83" s="8" t="s">
         <v>153</v>
       </c>
@@ -8050,7 +8050,7 @@
       <c r="U83" s="8"/>
     </row>
     <row r="84" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A84" s="91"/>
+      <c r="A84" s="93"/>
       <c r="B84" s="6">
         <v>45265</v>
       </c>
@@ -8063,7 +8063,7 @@
       <c r="E84" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="F84" s="91"/>
+      <c r="F84" s="93"/>
       <c r="G84" s="8" t="s">
         <v>154</v>
       </c>
@@ -8107,7 +8107,7 @@
       <c r="U84" s="8"/>
     </row>
     <row r="85" spans="1:21" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="91"/>
+      <c r="A85" s="93"/>
       <c r="B85" s="6">
         <v>45265</v>
       </c>
@@ -8120,7 +8120,7 @@
       <c r="E85" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="F85" s="91"/>
+      <c r="F85" s="93"/>
       <c r="G85" s="8" t="s">
         <v>155</v>
       </c>
@@ -8162,7 +8162,7 @@
       <c r="U85" s="8"/>
     </row>
     <row r="86" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="93" t="s">
+      <c r="A86" s="98" t="s">
         <v>157</v>
       </c>
       <c r="B86" s="3">
@@ -8177,7 +8177,7 @@
       <c r="E86" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F86" s="93" t="s">
+      <c r="F86" s="98" t="s">
         <v>174</v>
       </c>
       <c r="G86" s="2" t="s">
@@ -8223,7 +8223,7 @@
       <c r="U86" s="2"/>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A87" s="94"/>
+      <c r="A87" s="99"/>
       <c r="B87" s="3">
         <v>45337</v>
       </c>
@@ -8236,7 +8236,7 @@
       <c r="E87" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F87" s="94"/>
+      <c r="F87" s="99"/>
       <c r="G87" s="2" t="s">
         <v>159</v>
       </c>
@@ -8278,7 +8278,7 @@
       <c r="U87" s="2"/>
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A88" s="94"/>
+      <c r="A88" s="99"/>
       <c r="B88" s="3">
         <v>45337</v>
       </c>
@@ -8291,7 +8291,7 @@
       <c r="E88" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="F88" s="94"/>
+      <c r="F88" s="99"/>
       <c r="G88" s="2" t="s">
         <v>160</v>
       </c>
@@ -8335,7 +8335,7 @@
       <c r="U88" s="2"/>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A89" s="94"/>
+      <c r="A89" s="99"/>
       <c r="B89" s="3">
         <v>45337</v>
       </c>
@@ -8348,7 +8348,7 @@
       <c r="E89" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="F89" s="94"/>
+      <c r="F89" s="99"/>
       <c r="G89" s="2" t="s">
         <v>161</v>
       </c>
@@ -8390,7 +8390,7 @@
       <c r="U89" s="2"/>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A90" s="94"/>
+      <c r="A90" s="99"/>
       <c r="B90" s="3">
         <v>45337</v>
       </c>
@@ -8403,7 +8403,7 @@
       <c r="E90" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="F90" s="94"/>
+      <c r="F90" s="99"/>
       <c r="G90" s="2" t="s">
         <v>162</v>
       </c>
@@ -8447,7 +8447,7 @@
       <c r="U90" s="2"/>
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A91" s="94"/>
+      <c r="A91" s="99"/>
       <c r="B91" s="3">
         <v>45337</v>
       </c>
@@ -8460,7 +8460,7 @@
       <c r="E91" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="F91" s="94"/>
+      <c r="F91" s="99"/>
       <c r="G91" s="2" t="s">
         <v>163</v>
       </c>
@@ -8502,7 +8502,7 @@
       <c r="U91" s="2"/>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A92" s="94"/>
+      <c r="A92" s="99"/>
       <c r="B92" s="3">
         <v>45337</v>
       </c>
@@ -8515,7 +8515,7 @@
       <c r="E92" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="F92" s="94"/>
+      <c r="F92" s="99"/>
       <c r="G92" s="2" t="s">
         <v>164</v>
       </c>
@@ -8559,7 +8559,7 @@
       <c r="U92" s="2"/>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A93" s="95"/>
+      <c r="A93" s="100"/>
       <c r="B93" s="3">
         <v>45337</v>
       </c>
@@ -8572,7 +8572,7 @@
       <c r="E93" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="F93" s="95"/>
+      <c r="F93" s="100"/>
       <c r="G93" s="2" t="s">
         <v>165</v>
       </c>
@@ -8614,7 +8614,7 @@
       <c r="U93" s="2"/>
     </row>
     <row r="94" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="90" t="s">
+      <c r="A94" s="92" t="s">
         <v>166</v>
       </c>
       <c r="B94" s="6">
@@ -8625,7 +8625,7 @@
       </c>
       <c r="D94" s="8"/>
       <c r="E94" s="8"/>
-      <c r="F94" s="90" t="s">
+      <c r="F94" s="92" t="s">
         <v>178</v>
       </c>
       <c r="G94" s="8" t="s">
@@ -8671,7 +8671,7 @@
       <c r="U94" s="8"/>
     </row>
     <row r="95" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="91"/>
+      <c r="A95" s="93"/>
       <c r="B95" s="6">
         <v>45365</v>
       </c>
@@ -8680,7 +8680,7 @@
       </c>
       <c r="D95" s="8"/>
       <c r="E95" s="8"/>
-      <c r="F95" s="106"/>
+      <c r="F95" s="107"/>
       <c r="G95" s="8" t="s">
         <v>180</v>
       </c>
@@ -8722,7 +8722,7 @@
       <c r="U95" s="8"/>
     </row>
     <row r="96" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="91"/>
+      <c r="A96" s="93"/>
       <c r="B96" s="6">
         <v>45365</v>
       </c>
@@ -8731,7 +8731,7 @@
       </c>
       <c r="D96" s="8"/>
       <c r="E96" s="8"/>
-      <c r="F96" s="106"/>
+      <c r="F96" s="107"/>
       <c r="G96" s="8" t="s">
         <v>181</v>
       </c>
@@ -8775,7 +8775,7 @@
       <c r="U96" s="8"/>
     </row>
     <row r="97" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="91"/>
+      <c r="A97" s="93"/>
       <c r="B97" s="6">
         <v>45365</v>
       </c>
@@ -8784,7 +8784,7 @@
       </c>
       <c r="D97" s="8"/>
       <c r="E97" s="8"/>
-      <c r="F97" s="106"/>
+      <c r="F97" s="107"/>
       <c r="G97" s="8" t="s">
         <v>182</v>
       </c>
@@ -8826,7 +8826,7 @@
       <c r="U97" s="8"/>
     </row>
     <row r="98" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="91"/>
+      <c r="A98" s="93"/>
       <c r="B98" s="6">
         <v>45365</v>
       </c>
@@ -8839,7 +8839,7 @@
       <c r="E98" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="F98" s="106"/>
+      <c r="F98" s="107"/>
       <c r="G98" s="8" t="s">
         <v>183</v>
       </c>
@@ -8883,7 +8883,7 @@
       <c r="U98" s="8"/>
     </row>
     <row r="99" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="91"/>
+      <c r="A99" s="93"/>
       <c r="B99" s="6">
         <v>45365</v>
       </c>
@@ -8896,7 +8896,7 @@
       <c r="E99" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="F99" s="106"/>
+      <c r="F99" s="107"/>
       <c r="G99" s="8" t="s">
         <v>184</v>
       </c>
@@ -8938,7 +8938,7 @@
       <c r="U99" s="8"/>
     </row>
     <row r="100" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="91"/>
+      <c r="A100" s="93"/>
       <c r="B100" s="6">
         <v>45365</v>
       </c>
@@ -8951,7 +8951,7 @@
       <c r="E100" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="F100" s="106"/>
+      <c r="F100" s="107"/>
       <c r="G100" s="8" t="s">
         <v>185</v>
       </c>
@@ -8995,7 +8995,7 @@
       <c r="U100" s="8"/>
     </row>
     <row r="101" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="91"/>
+      <c r="A101" s="93"/>
       <c r="B101" s="6">
         <v>45365</v>
       </c>
@@ -9008,7 +9008,7 @@
       <c r="E101" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="F101" s="107"/>
+      <c r="F101" s="108"/>
       <c r="G101" s="8" t="s">
         <v>186</v>
       </c>
@@ -9050,7 +9050,7 @@
       <c r="U101" s="8"/>
     </row>
     <row r="102" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="93" t="s">
+      <c r="A102" s="98" t="s">
         <v>187</v>
       </c>
       <c r="B102" s="3">
@@ -9065,7 +9065,7 @@
       <c r="E102" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="F102" s="93" t="s">
+      <c r="F102" s="98" t="s">
         <v>188</v>
       </c>
       <c r="G102" s="2" t="s">
@@ -9111,7 +9111,7 @@
       <c r="U102" s="2"/>
     </row>
     <row r="103" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A103" s="94"/>
+      <c r="A103" s="99"/>
       <c r="B103" s="3">
         <v>45411</v>
       </c>
@@ -9124,7 +9124,7 @@
       <c r="E103" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="F103" s="94"/>
+      <c r="F103" s="99"/>
       <c r="G103" s="2" t="s">
         <v>194</v>
       </c>
@@ -9166,7 +9166,7 @@
       <c r="U103" s="2"/>
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A104" s="94"/>
+      <c r="A104" s="99"/>
       <c r="B104" s="3">
         <v>45411</v>
       </c>
@@ -9179,7 +9179,7 @@
       <c r="E104" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="F104" s="94"/>
+      <c r="F104" s="99"/>
       <c r="G104" s="2" t="s">
         <v>195</v>
       </c>
@@ -9223,7 +9223,7 @@
       <c r="U104" s="2"/>
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A105" s="94"/>
+      <c r="A105" s="99"/>
       <c r="B105" s="3">
         <v>45411</v>
       </c>
@@ -9236,7 +9236,7 @@
       <c r="E105" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="F105" s="94"/>
+      <c r="F105" s="99"/>
       <c r="G105" s="2" t="s">
         <v>196</v>
       </c>
@@ -9278,7 +9278,7 @@
       <c r="U105" s="2"/>
     </row>
     <row r="106" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A106" s="94"/>
+      <c r="A106" s="99"/>
       <c r="B106" s="3">
         <v>45411</v>
       </c>
@@ -9291,7 +9291,7 @@
       <c r="E106" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="F106" s="94"/>
+      <c r="F106" s="99"/>
       <c r="G106" s="2" t="s">
         <v>197</v>
       </c>
@@ -9335,7 +9335,7 @@
       <c r="U106" s="2"/>
     </row>
     <row r="107" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A107" s="94"/>
+      <c r="A107" s="99"/>
       <c r="B107" s="3">
         <v>45411</v>
       </c>
@@ -9348,7 +9348,7 @@
       <c r="E107" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="F107" s="94"/>
+      <c r="F107" s="99"/>
       <c r="G107" s="2" t="s">
         <v>198</v>
       </c>
@@ -9390,7 +9390,7 @@
       <c r="U107" s="2"/>
     </row>
     <row r="108" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A108" s="94"/>
+      <c r="A108" s="99"/>
       <c r="B108" s="3">
         <v>45411</v>
       </c>
@@ -9403,7 +9403,7 @@
       <c r="E108" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="F108" s="94"/>
+      <c r="F108" s="99"/>
       <c r="G108" s="2" t="s">
         <v>199</v>
       </c>
@@ -9447,7 +9447,7 @@
       <c r="U108" s="2"/>
     </row>
     <row r="109" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A109" s="94"/>
+      <c r="A109" s="99"/>
       <c r="B109" s="3">
         <v>45411</v>
       </c>
@@ -9460,7 +9460,7 @@
       <c r="E109" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="F109" s="94"/>
+      <c r="F109" s="99"/>
       <c r="G109" s="2" t="s">
         <v>200</v>
       </c>
@@ -9502,7 +9502,7 @@
       <c r="U109" s="2"/>
     </row>
     <row r="110" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A110" s="94"/>
+      <c r="A110" s="99"/>
       <c r="B110" s="3">
         <v>45411</v>
       </c>
@@ -9515,7 +9515,7 @@
       <c r="E110" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="F110" s="94"/>
+      <c r="F110" s="99"/>
       <c r="G110" s="2" t="s">
         <v>201</v>
       </c>
@@ -9559,7 +9559,7 @@
       <c r="U110" s="2"/>
     </row>
     <row r="111" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A111" s="94"/>
+      <c r="A111" s="99"/>
       <c r="B111" s="3">
         <v>45411</v>
       </c>
@@ -9572,7 +9572,7 @@
       <c r="E111" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="F111" s="94"/>
+      <c r="F111" s="99"/>
       <c r="G111" s="2" t="s">
         <v>202</v>
       </c>
@@ -9614,7 +9614,7 @@
       <c r="U111" s="2"/>
     </row>
     <row r="112" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A112" s="94"/>
+      <c r="A112" s="99"/>
       <c r="B112" s="3">
         <v>45411</v>
       </c>
@@ -9627,7 +9627,7 @@
       <c r="E112" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="F112" s="94"/>
+      <c r="F112" s="99"/>
       <c r="G112" s="2" t="s">
         <v>203</v>
       </c>
@@ -9671,7 +9671,7 @@
       <c r="U112" s="2"/>
     </row>
     <row r="113" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A113" s="95"/>
+      <c r="A113" s="100"/>
       <c r="B113" s="3">
         <v>45411</v>
       </c>
@@ -9684,7 +9684,7 @@
       <c r="E113" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="F113" s="95"/>
+      <c r="F113" s="100"/>
       <c r="G113" s="2" t="s">
         <v>204</v>
       </c>
@@ -9726,7 +9726,7 @@
       <c r="U113" s="2"/>
     </row>
     <row r="114" spans="1:21" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="90" t="s">
+      <c r="A114" s="92" t="s">
         <v>205</v>
       </c>
       <c r="B114" s="6">
@@ -9741,7 +9741,7 @@
       <c r="E114" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="F114" s="90" t="s">
+      <c r="F114" s="92" t="s">
         <v>210</v>
       </c>
       <c r="G114" s="8" t="s">
@@ -9785,7 +9785,7 @@
       </c>
     </row>
     <row r="115" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="91"/>
+      <c r="A115" s="93"/>
       <c r="B115" s="6">
         <v>45441</v>
       </c>
@@ -9798,7 +9798,7 @@
       <c r="E115" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="F115" s="91"/>
+      <c r="F115" s="93"/>
       <c r="G115" s="8" t="s">
         <v>213</v>
       </c>
@@ -9840,7 +9840,7 @@
       <c r="U115" s="8"/>
     </row>
     <row r="116" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="91"/>
+      <c r="A116" s="93"/>
       <c r="B116" s="6">
         <v>45441</v>
       </c>
@@ -9853,7 +9853,7 @@
       <c r="E116" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="F116" s="91"/>
+      <c r="F116" s="93"/>
       <c r="G116" s="8" t="s">
         <v>211</v>
       </c>
@@ -9895,7 +9895,7 @@
       <c r="U116" s="8"/>
     </row>
     <row r="117" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="91"/>
+      <c r="A117" s="93"/>
       <c r="B117" s="6">
         <v>45441</v>
       </c>
@@ -9908,7 +9908,7 @@
       <c r="E117" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="F117" s="91"/>
+      <c r="F117" s="93"/>
       <c r="G117" s="8" t="s">
         <v>214</v>
       </c>
@@ -9948,7 +9948,7 @@
       <c r="U117" s="8"/>
     </row>
     <row r="118" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="91"/>
+      <c r="A118" s="93"/>
       <c r="B118" s="6">
         <v>45441</v>
       </c>
@@ -9961,7 +9961,7 @@
       <c r="E118" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="F118" s="91"/>
+      <c r="F118" s="93"/>
       <c r="G118" s="8" t="s">
         <v>215</v>
       </c>
@@ -10003,7 +10003,7 @@
       <c r="U118" s="8"/>
     </row>
     <row r="119" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="91"/>
+      <c r="A119" s="93"/>
       <c r="B119" s="6">
         <v>45441</v>
       </c>
@@ -10016,7 +10016,7 @@
       <c r="E119" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="F119" s="91"/>
+      <c r="F119" s="93"/>
       <c r="G119" s="8" t="s">
         <v>216</v>
       </c>
@@ -10056,7 +10056,7 @@
       <c r="U119" s="8"/>
     </row>
     <row r="120" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="91"/>
+      <c r="A120" s="93"/>
       <c r="B120" s="6">
         <v>45441</v>
       </c>
@@ -10069,7 +10069,7 @@
       <c r="E120" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="F120" s="91"/>
+      <c r="F120" s="93"/>
       <c r="G120" s="8" t="s">
         <v>219</v>
       </c>
@@ -10111,7 +10111,7 @@
       <c r="U120" s="8"/>
     </row>
     <row r="121" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="91"/>
+      <c r="A121" s="93"/>
       <c r="B121" s="6">
         <v>45441</v>
       </c>
@@ -10124,7 +10124,7 @@
       <c r="E121" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="F121" s="91"/>
+      <c r="F121" s="93"/>
       <c r="G121" s="8" t="s">
         <v>220</v>
       </c>
@@ -10164,7 +10164,7 @@
       <c r="U121" s="8"/>
     </row>
     <row r="122" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="91"/>
+      <c r="A122" s="93"/>
       <c r="B122" s="6">
         <v>45441</v>
       </c>
@@ -10177,7 +10177,7 @@
       <c r="E122" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="F122" s="91"/>
+      <c r="F122" s="93"/>
       <c r="G122" s="8" t="s">
         <v>217</v>
       </c>
@@ -10219,7 +10219,7 @@
       <c r="U122" s="8"/>
     </row>
     <row r="123" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="91"/>
+      <c r="A123" s="93"/>
       <c r="B123" s="6">
         <v>45441</v>
       </c>
@@ -10232,7 +10232,7 @@
       <c r="E123" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="F123" s="91"/>
+      <c r="F123" s="93"/>
       <c r="G123" s="8" t="s">
         <v>218</v>
       </c>
@@ -10272,7 +10272,7 @@
       <c r="U123" s="8"/>
     </row>
     <row r="124" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="91"/>
+      <c r="A124" s="93"/>
       <c r="B124" s="6">
         <v>45441</v>
       </c>
@@ -10285,7 +10285,7 @@
       <c r="E124" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="F124" s="91"/>
+      <c r="F124" s="93"/>
       <c r="G124" s="8" t="s">
         <v>221</v>
       </c>
@@ -10327,7 +10327,7 @@
       <c r="U124" s="8"/>
     </row>
     <row r="125" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="92"/>
+      <c r="A125" s="94"/>
       <c r="B125" s="6">
         <v>45441</v>
       </c>
@@ -10340,7 +10340,7 @@
       <c r="E125" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="F125" s="92"/>
+      <c r="F125" s="94"/>
       <c r="G125" s="8" t="s">
         <v>222</v>
       </c>
@@ -10380,7 +10380,7 @@
       <c r="U125" s="8"/>
     </row>
     <row r="126" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A126" s="93" t="s">
+      <c r="A126" s="98" t="s">
         <v>236</v>
       </c>
       <c r="B126" s="3">
@@ -10395,7 +10395,7 @@
       <c r="E126" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="F126" s="97" t="s">
+      <c r="F126" s="101" t="s">
         <v>241</v>
       </c>
       <c r="G126" s="12" t="s">
@@ -10439,7 +10439,7 @@
       <c r="U126" s="2"/>
     </row>
     <row r="127" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A127" s="94"/>
+      <c r="A127" s="99"/>
       <c r="B127" s="3">
         <v>45455</v>
       </c>
@@ -10452,7 +10452,7 @@
       <c r="E127" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="F127" s="98"/>
+      <c r="F127" s="102"/>
       <c r="G127" s="12" t="s">
         <v>225</v>
       </c>
@@ -10492,7 +10492,7 @@
       <c r="U127" s="2"/>
     </row>
     <row r="128" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A128" s="94"/>
+      <c r="A128" s="99"/>
       <c r="B128" s="3">
         <v>45455</v>
       </c>
@@ -10505,7 +10505,7 @@
       <c r="E128" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="F128" s="98"/>
+      <c r="F128" s="102"/>
       <c r="G128" s="12" t="s">
         <v>226</v>
       </c>
@@ -10547,7 +10547,7 @@
       <c r="U128" s="2"/>
     </row>
     <row r="129" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A129" s="94"/>
+      <c r="A129" s="99"/>
       <c r="B129" s="3">
         <v>45455</v>
       </c>
@@ -10560,7 +10560,7 @@
       <c r="E129" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="F129" s="98"/>
+      <c r="F129" s="102"/>
       <c r="G129" s="12" t="s">
         <v>227</v>
       </c>
@@ -10600,7 +10600,7 @@
       <c r="U129" s="2"/>
     </row>
     <row r="130" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A130" s="94"/>
+      <c r="A130" s="99"/>
       <c r="B130" s="3">
         <v>45455</v>
       </c>
@@ -10613,7 +10613,7 @@
       <c r="E130" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="F130" s="98"/>
+      <c r="F130" s="102"/>
       <c r="G130" s="12" t="s">
         <v>228</v>
       </c>
@@ -10655,7 +10655,7 @@
       <c r="U130" s="2"/>
     </row>
     <row r="131" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A131" s="94"/>
+      <c r="A131" s="99"/>
       <c r="B131" s="3">
         <v>45455</v>
       </c>
@@ -10668,7 +10668,7 @@
       <c r="E131" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="F131" s="98"/>
+      <c r="F131" s="102"/>
       <c r="G131" s="12" t="s">
         <v>229</v>
       </c>
@@ -10710,7 +10710,7 @@
       </c>
     </row>
     <row r="132" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A132" s="94"/>
+      <c r="A132" s="99"/>
       <c r="B132" s="3">
         <v>45455</v>
       </c>
@@ -10723,7 +10723,7 @@
       <c r="E132" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="F132" s="98"/>
+      <c r="F132" s="102"/>
       <c r="G132" s="12" t="s">
         <v>230</v>
       </c>
@@ -10765,7 +10765,7 @@
       <c r="U132" s="2"/>
     </row>
     <row r="133" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A133" s="94"/>
+      <c r="A133" s="99"/>
       <c r="B133" s="3">
         <v>45455</v>
       </c>
@@ -10778,7 +10778,7 @@
       <c r="E133" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="F133" s="98"/>
+      <c r="F133" s="102"/>
       <c r="G133" s="12" t="s">
         <v>231</v>
       </c>
@@ -10818,7 +10818,7 @@
       <c r="U133" s="2"/>
     </row>
     <row r="134" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A134" s="94"/>
+      <c r="A134" s="99"/>
       <c r="B134" s="3">
         <v>45455</v>
       </c>
@@ -10831,7 +10831,7 @@
       <c r="E134" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="F134" s="98"/>
+      <c r="F134" s="102"/>
       <c r="G134" s="12" t="s">
         <v>232</v>
       </c>
@@ -10873,7 +10873,7 @@
       <c r="U134" s="2"/>
     </row>
     <row r="135" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A135" s="94"/>
+      <c r="A135" s="99"/>
       <c r="B135" s="3">
         <v>45455</v>
       </c>
@@ -10886,7 +10886,7 @@
       <c r="E135" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="F135" s="98"/>
+      <c r="F135" s="102"/>
       <c r="G135" s="12" t="s">
         <v>233</v>
       </c>
@@ -10928,7 +10928,7 @@
       </c>
     </row>
     <row r="136" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A136" s="94"/>
+      <c r="A136" s="99"/>
       <c r="B136" s="3">
         <v>45455</v>
       </c>
@@ -10941,7 +10941,7 @@
       <c r="E136" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="F136" s="98"/>
+      <c r="F136" s="102"/>
       <c r="G136" s="12" t="s">
         <v>234</v>
       </c>
@@ -10983,7 +10983,7 @@
       <c r="U136" s="2"/>
     </row>
     <row r="137" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A137" s="95"/>
+      <c r="A137" s="100"/>
       <c r="B137" s="3">
         <v>45455</v>
       </c>
@@ -10996,7 +10996,7 @@
       <c r="E137" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="F137" s="99"/>
+      <c r="F137" s="103"/>
       <c r="G137" s="12" t="s">
         <v>235</v>
       </c>
@@ -11038,7 +11038,7 @@
       </c>
     </row>
     <row r="138" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A138" s="90" t="s">
+      <c r="A138" s="92" t="s">
         <v>243</v>
       </c>
       <c r="B138" s="6">
@@ -11053,7 +11053,7 @@
       <c r="E138" s="8" t="s">
         <v>274</v>
       </c>
-      <c r="F138" s="100" t="s">
+      <c r="F138" s="95" t="s">
         <v>271</v>
       </c>
       <c r="G138" s="8" t="s">
@@ -11097,7 +11097,7 @@
       <c r="U138" s="8"/>
     </row>
     <row r="139" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A139" s="91"/>
+      <c r="A139" s="93"/>
       <c r="B139" s="6">
         <v>45482</v>
       </c>
@@ -11110,7 +11110,7 @@
       <c r="E139" s="8" t="s">
         <v>274</v>
       </c>
-      <c r="F139" s="101"/>
+      <c r="F139" s="96"/>
       <c r="G139" s="8" t="s">
         <v>248</v>
       </c>
@@ -11150,7 +11150,7 @@
       <c r="U139" s="8"/>
     </row>
     <row r="140" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A140" s="91"/>
+      <c r="A140" s="93"/>
       <c r="B140" s="6">
         <v>45482</v>
       </c>
@@ -11163,7 +11163,7 @@
       <c r="E140" s="8" t="s">
         <v>274</v>
       </c>
-      <c r="F140" s="101"/>
+      <c r="F140" s="96"/>
       <c r="G140" s="8" t="s">
         <v>245</v>
       </c>
@@ -11205,7 +11205,7 @@
       <c r="U140" s="8"/>
     </row>
     <row r="141" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A141" s="91"/>
+      <c r="A141" s="93"/>
       <c r="B141" s="6">
         <v>45482</v>
       </c>
@@ -11218,7 +11218,7 @@
       <c r="E141" s="8" t="s">
         <v>274</v>
       </c>
-      <c r="F141" s="101"/>
+      <c r="F141" s="96"/>
       <c r="G141" s="8" t="s">
         <v>246</v>
       </c>
@@ -11258,14 +11258,14 @@
       <c r="U141" s="8"/>
     </row>
     <row r="142" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A142" s="91"/>
+      <c r="A142" s="93"/>
       <c r="B142" s="6">
         <v>45482</v>
       </c>
       <c r="C142" s="7"/>
       <c r="D142" s="8"/>
       <c r="E142" s="8"/>
-      <c r="F142" s="101"/>
+      <c r="F142" s="96"/>
       <c r="G142" s="8" t="s">
         <v>242</v>
       </c>
@@ -11307,14 +11307,14 @@
       <c r="U142" s="8"/>
     </row>
     <row r="143" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A143" s="91"/>
+      <c r="A143" s="93"/>
       <c r="B143" s="6">
         <v>45482</v>
       </c>
       <c r="C143" s="7"/>
       <c r="D143" s="8"/>
       <c r="E143" s="8"/>
-      <c r="F143" s="101"/>
+      <c r="F143" s="96"/>
       <c r="G143" s="8" t="s">
         <v>244</v>
       </c>
@@ -11354,7 +11354,7 @@
       <c r="U143" s="8"/>
     </row>
     <row r="144" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A144" s="91"/>
+      <c r="A144" s="93"/>
       <c r="B144" s="6">
         <v>45482</v>
       </c>
@@ -11367,7 +11367,7 @@
       <c r="E144" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="F144" s="101"/>
+      <c r="F144" s="96"/>
       <c r="G144" s="8" t="s">
         <v>253</v>
       </c>
@@ -11409,7 +11409,7 @@
       <c r="U144" s="8"/>
     </row>
     <row r="145" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A145" s="91"/>
+      <c r="A145" s="93"/>
       <c r="B145" s="6">
         <v>45482</v>
       </c>
@@ -11422,7 +11422,7 @@
       <c r="E145" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="F145" s="101"/>
+      <c r="F145" s="96"/>
       <c r="G145" s="8" t="s">
         <v>254</v>
       </c>
@@ -11462,7 +11462,7 @@
       <c r="U145" s="8"/>
     </row>
     <row r="146" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A146" s="91"/>
+      <c r="A146" s="93"/>
       <c r="B146" s="6">
         <v>45482</v>
       </c>
@@ -11475,7 +11475,7 @@
       <c r="E146" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="F146" s="101"/>
+      <c r="F146" s="96"/>
       <c r="G146" s="8" t="s">
         <v>251</v>
       </c>
@@ -11517,7 +11517,7 @@
       <c r="U146" s="8"/>
     </row>
     <row r="147" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A147" s="91"/>
+      <c r="A147" s="93"/>
       <c r="B147" s="6">
         <v>45482</v>
       </c>
@@ -11530,7 +11530,7 @@
       <c r="E147" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="F147" s="101"/>
+      <c r="F147" s="96"/>
       <c r="G147" s="8" t="s">
         <v>252</v>
       </c>
@@ -11570,14 +11570,14 @@
       <c r="U147" s="8"/>
     </row>
     <row r="148" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A148" s="91"/>
+      <c r="A148" s="93"/>
       <c r="B148" s="6">
         <v>45482</v>
       </c>
       <c r="C148" s="7"/>
       <c r="D148" s="8"/>
       <c r="E148" s="8"/>
-      <c r="F148" s="101"/>
+      <c r="F148" s="96"/>
       <c r="G148" s="8" t="s">
         <v>249</v>
       </c>
@@ -11619,14 +11619,14 @@
       <c r="U148" s="8"/>
     </row>
     <row r="149" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A149" s="92"/>
+      <c r="A149" s="94"/>
       <c r="B149" s="6">
         <v>45482</v>
       </c>
       <c r="C149" s="7"/>
       <c r="D149" s="8"/>
       <c r="E149" s="8"/>
-      <c r="F149" s="112"/>
+      <c r="F149" s="97"/>
       <c r="G149" s="8" t="s">
         <v>250</v>
       </c>
@@ -11666,7 +11666,7 @@
       <c r="U149" s="8"/>
     </row>
     <row r="150" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A150" s="93" t="s">
+      <c r="A150" s="98" t="s">
         <v>255</v>
       </c>
       <c r="B150" s="3">
@@ -11681,7 +11681,7 @@
       <c r="E150" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="F150" s="97" t="s">
+      <c r="F150" s="101" t="s">
         <v>270</v>
       </c>
       <c r="G150" s="12" t="s">
@@ -11725,7 +11725,7 @@
       <c r="U150" s="2"/>
     </row>
     <row r="151" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A151" s="94"/>
+      <c r="A151" s="99"/>
       <c r="B151" s="3">
         <v>45496</v>
       </c>
@@ -11738,7 +11738,7 @@
       <c r="E151" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="F151" s="98"/>
+      <c r="F151" s="102"/>
       <c r="G151" s="12" t="s">
         <v>257</v>
       </c>
@@ -11778,7 +11778,7 @@
       <c r="U151" s="2"/>
     </row>
     <row r="152" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A152" s="94"/>
+      <c r="A152" s="99"/>
       <c r="B152" s="3">
         <v>45496</v>
       </c>
@@ -11791,7 +11791,7 @@
       <c r="E152" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="F152" s="98"/>
+      <c r="F152" s="102"/>
       <c r="G152" s="12" t="s">
         <v>258</v>
       </c>
@@ -11833,7 +11833,7 @@
       <c r="U152" s="2"/>
     </row>
     <row r="153" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A153" s="94"/>
+      <c r="A153" s="99"/>
       <c r="B153" s="3">
         <v>45496</v>
       </c>
@@ -11846,7 +11846,7 @@
       <c r="E153" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="F153" s="98"/>
+      <c r="F153" s="102"/>
       <c r="G153" s="12" t="s">
         <v>259</v>
       </c>
@@ -11886,7 +11886,7 @@
       <c r="U153" s="2"/>
     </row>
     <row r="154" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A154" s="94"/>
+      <c r="A154" s="99"/>
       <c r="B154" s="3">
         <v>45496</v>
       </c>
@@ -11899,7 +11899,7 @@
       <c r="E154" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="F154" s="98"/>
+      <c r="F154" s="102"/>
       <c r="G154" s="12" t="s">
         <v>260</v>
       </c>
@@ -11941,7 +11941,7 @@
       <c r="U154" s="2"/>
     </row>
     <row r="155" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A155" s="94"/>
+      <c r="A155" s="99"/>
       <c r="B155" s="3">
         <v>45496</v>
       </c>
@@ -11954,7 +11954,7 @@
       <c r="E155" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="F155" s="98"/>
+      <c r="F155" s="102"/>
       <c r="G155" s="12" t="s">
         <v>261</v>
       </c>
@@ -11994,7 +11994,7 @@
       <c r="U155" s="2"/>
     </row>
     <row r="156" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A156" s="94"/>
+      <c r="A156" s="99"/>
       <c r="B156" s="3">
         <v>45496</v>
       </c>
@@ -12007,7 +12007,7 @@
       <c r="E156" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="F156" s="98"/>
+      <c r="F156" s="102"/>
       <c r="G156" s="12" t="s">
         <v>262</v>
       </c>
@@ -12049,7 +12049,7 @@
       <c r="U156" s="2"/>
     </row>
     <row r="157" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A157" s="94"/>
+      <c r="A157" s="99"/>
       <c r="B157" s="3">
         <v>45496</v>
       </c>
@@ -12062,7 +12062,7 @@
       <c r="E157" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="F157" s="98"/>
+      <c r="F157" s="102"/>
       <c r="G157" s="12" t="s">
         <v>263</v>
       </c>
@@ -12102,7 +12102,7 @@
       <c r="U157" s="2"/>
     </row>
     <row r="158" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A158" s="94"/>
+      <c r="A158" s="99"/>
       <c r="B158" s="3">
         <v>45496</v>
       </c>
@@ -12115,7 +12115,7 @@
       <c r="E158" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="F158" s="98"/>
+      <c r="F158" s="102"/>
       <c r="G158" s="12" t="s">
         <v>264</v>
       </c>
@@ -12157,7 +12157,7 @@
       <c r="U158" s="2"/>
     </row>
     <row r="159" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A159" s="94"/>
+      <c r="A159" s="99"/>
       <c r="B159" s="3">
         <v>45496</v>
       </c>
@@ -12170,7 +12170,7 @@
       <c r="E159" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="F159" s="98"/>
+      <c r="F159" s="102"/>
       <c r="G159" s="12" t="s">
         <v>265</v>
       </c>
@@ -12210,7 +12210,7 @@
       <c r="U159" s="2"/>
     </row>
     <row r="160" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A160" s="94"/>
+      <c r="A160" s="99"/>
       <c r="B160" s="3">
         <v>45496</v>
       </c>
@@ -12223,7 +12223,7 @@
       <c r="E160" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="F160" s="98"/>
+      <c r="F160" s="102"/>
       <c r="G160" s="12" t="s">
         <v>266</v>
       </c>
@@ -12265,7 +12265,7 @@
       <c r="U160" s="2"/>
     </row>
     <row r="161" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A161" s="95"/>
+      <c r="A161" s="100"/>
       <c r="B161" s="3">
         <v>45496</v>
       </c>
@@ -12278,7 +12278,7 @@
       <c r="E161" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="F161" s="99"/>
+      <c r="F161" s="103"/>
       <c r="G161" s="12" t="s">
         <v>267</v>
       </c>
@@ -12318,7 +12318,7 @@
       <c r="U161" s="2"/>
     </row>
     <row r="162" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A162" s="90" t="s">
+      <c r="A162" s="92" t="s">
         <v>277</v>
       </c>
       <c r="B162" s="6">
@@ -12333,7 +12333,7 @@
       <c r="E162" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="F162" s="100" t="s">
+      <c r="F162" s="95" t="s">
         <v>280</v>
       </c>
       <c r="G162" s="13" t="s">
@@ -12377,7 +12377,7 @@
       <c r="U162" s="8"/>
     </row>
     <row r="163" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A163" s="91"/>
+      <c r="A163" s="93"/>
       <c r="B163" s="6">
         <v>45519</v>
       </c>
@@ -12390,7 +12390,7 @@
       <c r="E163" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="F163" s="101"/>
+      <c r="F163" s="96"/>
       <c r="G163" s="13" t="s">
         <v>282</v>
       </c>
@@ -12430,7 +12430,7 @@
       <c r="U163" s="8"/>
     </row>
     <row r="164" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A164" s="91"/>
+      <c r="A164" s="93"/>
       <c r="B164" s="6">
         <v>45519</v>
       </c>
@@ -12443,7 +12443,7 @@
       <c r="E164" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="F164" s="101"/>
+      <c r="F164" s="96"/>
       <c r="G164" s="13" t="s">
         <v>283</v>
       </c>
@@ -12485,7 +12485,7 @@
       <c r="U164" s="8"/>
     </row>
     <row r="165" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A165" s="91"/>
+      <c r="A165" s="93"/>
       <c r="B165" s="6">
         <v>45519</v>
       </c>
@@ -12498,7 +12498,7 @@
       <c r="E165" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="F165" s="101"/>
+      <c r="F165" s="96"/>
       <c r="G165" s="13" t="s">
         <v>284</v>
       </c>
@@ -12538,7 +12538,7 @@
       <c r="U165" s="8"/>
     </row>
     <row r="166" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A166" s="91"/>
+      <c r="A166" s="93"/>
       <c r="B166" s="6">
         <v>45519</v>
       </c>
@@ -12551,7 +12551,7 @@
       <c r="E166" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="F166" s="101"/>
+      <c r="F166" s="96"/>
       <c r="G166" s="13" t="s">
         <v>285</v>
       </c>
@@ -12593,7 +12593,7 @@
       <c r="U166" s="8"/>
     </row>
     <row r="167" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A167" s="91"/>
+      <c r="A167" s="93"/>
       <c r="B167" s="6">
         <v>45519</v>
       </c>
@@ -12606,7 +12606,7 @@
       <c r="E167" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="F167" s="101"/>
+      <c r="F167" s="96"/>
       <c r="G167" s="13" t="s">
         <v>286</v>
       </c>
@@ -12646,7 +12646,7 @@
       <c r="U167" s="8"/>
     </row>
     <row r="168" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A168" s="91"/>
+      <c r="A168" s="93"/>
       <c r="B168" s="6">
         <v>45519</v>
       </c>
@@ -12659,7 +12659,7 @@
       <c r="E168" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="F168" s="101"/>
+      <c r="F168" s="96"/>
       <c r="G168" s="13" t="s">
         <v>287</v>
       </c>
@@ -12701,7 +12701,7 @@
       <c r="U168" s="8"/>
     </row>
     <row r="169" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A169" s="91"/>
+      <c r="A169" s="93"/>
       <c r="B169" s="6">
         <v>45519</v>
       </c>
@@ -12714,7 +12714,7 @@
       <c r="E169" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="F169" s="101"/>
+      <c r="F169" s="96"/>
       <c r="G169" s="13" t="s">
         <v>288</v>
       </c>
@@ -12754,7 +12754,7 @@
       <c r="U169" s="8"/>
     </row>
     <row r="170" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A170" s="93" t="s">
+      <c r="A170" s="98" t="s">
         <v>289</v>
       </c>
       <c r="B170" s="3">
@@ -12769,7 +12769,7 @@
       <c r="E170" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="F170" s="97" t="s">
+      <c r="F170" s="101" t="s">
         <v>294</v>
       </c>
       <c r="G170" s="12" t="s">
@@ -12813,7 +12813,7 @@
       <c r="U170" s="2"/>
     </row>
     <row r="171" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A171" s="94"/>
+      <c r="A171" s="99"/>
       <c r="B171" s="3">
         <v>45527</v>
       </c>
@@ -12826,7 +12826,7 @@
       <c r="E171" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="F171" s="98"/>
+      <c r="F171" s="102"/>
       <c r="G171" s="12" t="s">
         <v>296</v>
       </c>
@@ -12866,7 +12866,7 @@
       <c r="U171" s="2"/>
     </row>
     <row r="172" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A172" s="94"/>
+      <c r="A172" s="99"/>
       <c r="B172" s="3">
         <v>45527</v>
       </c>
@@ -12879,7 +12879,7 @@
       <c r="E172" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="F172" s="98"/>
+      <c r="F172" s="102"/>
       <c r="G172" s="12" t="s">
         <v>297</v>
       </c>
@@ -12921,7 +12921,7 @@
       <c r="U172" s="2"/>
     </row>
     <row r="173" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A173" s="94"/>
+      <c r="A173" s="99"/>
       <c r="B173" s="3">
         <v>45527</v>
       </c>
@@ -12934,7 +12934,7 @@
       <c r="E173" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="F173" s="98"/>
+      <c r="F173" s="102"/>
       <c r="G173" s="12" t="s">
         <v>298</v>
       </c>
@@ -12974,7 +12974,7 @@
       <c r="U173" s="2"/>
     </row>
     <row r="174" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A174" s="94"/>
+      <c r="A174" s="99"/>
       <c r="B174" s="3">
         <v>45527</v>
       </c>
@@ -12987,7 +12987,7 @@
       <c r="E174" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="F174" s="98"/>
+      <c r="F174" s="102"/>
       <c r="G174" s="12" t="s">
         <v>299</v>
       </c>
@@ -13029,7 +13029,7 @@
       <c r="U174" s="2"/>
     </row>
     <row r="175" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A175" s="94"/>
+      <c r="A175" s="99"/>
       <c r="B175" s="3">
         <v>45527</v>
       </c>
@@ -13042,7 +13042,7 @@
       <c r="E175" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="F175" s="98"/>
+      <c r="F175" s="102"/>
       <c r="G175" s="12" t="s">
         <v>300</v>
       </c>
@@ -13082,7 +13082,7 @@
       <c r="U175" s="2"/>
     </row>
     <row r="176" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A176" s="94"/>
+      <c r="A176" s="99"/>
       <c r="B176" s="3">
         <v>45527</v>
       </c>
@@ -13095,7 +13095,7 @@
       <c r="E176" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="F176" s="98"/>
+      <c r="F176" s="102"/>
       <c r="G176" s="12" t="s">
         <v>301</v>
       </c>
@@ -13137,7 +13137,7 @@
       <c r="U176" s="2"/>
     </row>
     <row r="177" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A177" s="94"/>
+      <c r="A177" s="99"/>
       <c r="B177" s="3">
         <v>45527</v>
       </c>
@@ -13150,7 +13150,7 @@
       <c r="E177" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="F177" s="98"/>
+      <c r="F177" s="102"/>
       <c r="G177" s="12" t="s">
         <v>302</v>
       </c>
@@ -13190,7 +13190,7 @@
       <c r="U177" s="2"/>
     </row>
     <row r="178" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A178" s="94"/>
+      <c r="A178" s="99"/>
       <c r="B178" s="3">
         <v>45527</v>
       </c>
@@ -13203,7 +13203,7 @@
       <c r="E178" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="F178" s="98"/>
+      <c r="F178" s="102"/>
       <c r="G178" s="12" t="s">
         <v>303</v>
       </c>
@@ -13245,7 +13245,7 @@
       <c r="U178" s="2"/>
     </row>
     <row r="179" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A179" s="94"/>
+      <c r="A179" s="99"/>
       <c r="B179" s="3">
         <v>45527</v>
       </c>
@@ -13258,7 +13258,7 @@
       <c r="E179" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="F179" s="98"/>
+      <c r="F179" s="102"/>
       <c r="G179" s="12" t="s">
         <v>304</v>
       </c>
@@ -13298,7 +13298,7 @@
       <c r="U179" s="2"/>
     </row>
     <row r="180" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A180" s="94"/>
+      <c r="A180" s="99"/>
       <c r="B180" s="3">
         <v>45527</v>
       </c>
@@ -13311,7 +13311,7 @@
       <c r="E180" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="F180" s="98"/>
+      <c r="F180" s="102"/>
       <c r="G180" s="12" t="s">
         <v>305</v>
       </c>
@@ -13353,7 +13353,7 @@
       <c r="U180" s="2"/>
     </row>
     <row r="181" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A181" s="95"/>
+      <c r="A181" s="100"/>
       <c r="B181" s="3">
         <v>45527</v>
       </c>
@@ -13366,7 +13366,7 @@
       <c r="E181" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="F181" s="99"/>
+      <c r="F181" s="103"/>
       <c r="G181" s="12" t="s">
         <v>306</v>
       </c>
@@ -13406,7 +13406,7 @@
       <c r="U181" s="2"/>
     </row>
     <row r="182" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A182" s="88" t="s">
+      <c r="A182" s="104" t="s">
         <v>307</v>
       </c>
       <c r="B182" s="6">
@@ -13421,7 +13421,7 @@
       <c r="E182" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="F182" s="88" t="s">
+      <c r="F182" s="104" t="s">
         <v>312</v>
       </c>
       <c r="G182" s="8" t="s">
@@ -13465,7 +13465,7 @@
       <c r="U182" s="8"/>
     </row>
     <row r="183" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A183" s="89"/>
+      <c r="A183" s="105"/>
       <c r="B183" s="6">
         <v>45539</v>
       </c>
@@ -13478,7 +13478,7 @@
       <c r="E183" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="F183" s="89"/>
+      <c r="F183" s="105"/>
       <c r="G183" s="8" t="s">
         <v>314</v>
       </c>
@@ -13518,7 +13518,7 @@
       <c r="U183" s="8"/>
     </row>
     <row r="184" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A184" s="89"/>
+      <c r="A184" s="105"/>
       <c r="B184" s="6">
         <v>45539</v>
       </c>
@@ -13531,7 +13531,7 @@
       <c r="E184" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="F184" s="89"/>
+      <c r="F184" s="105"/>
       <c r="G184" s="8" t="s">
         <v>315</v>
       </c>
@@ -13573,7 +13573,7 @@
       <c r="U184" s="8"/>
     </row>
     <row r="185" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A185" s="89"/>
+      <c r="A185" s="105"/>
       <c r="B185" s="6">
         <v>45539</v>
       </c>
@@ -13586,7 +13586,7 @@
       <c r="E185" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="F185" s="89"/>
+      <c r="F185" s="105"/>
       <c r="G185" s="8" t="s">
         <v>316</v>
       </c>
@@ -13626,7 +13626,7 @@
       <c r="U185" s="8"/>
     </row>
     <row r="186" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A186" s="89"/>
+      <c r="A186" s="105"/>
       <c r="B186" s="6">
         <v>45539</v>
       </c>
@@ -13639,7 +13639,7 @@
       <c r="E186" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="F186" s="89"/>
+      <c r="F186" s="105"/>
       <c r="G186" s="8" t="s">
         <v>317</v>
       </c>
@@ -13681,7 +13681,7 @@
       <c r="U186" s="8"/>
     </row>
     <row r="187" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A187" s="89"/>
+      <c r="A187" s="105"/>
       <c r="B187" s="6">
         <v>45539</v>
       </c>
@@ -13694,7 +13694,7 @@
       <c r="E187" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="F187" s="89"/>
+      <c r="F187" s="105"/>
       <c r="G187" s="8" t="s">
         <v>318</v>
       </c>
@@ -13734,7 +13734,7 @@
       <c r="U187" s="8"/>
     </row>
     <row r="188" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A188" s="89"/>
+      <c r="A188" s="105"/>
       <c r="B188" s="6">
         <v>45539</v>
       </c>
@@ -13747,7 +13747,7 @@
       <c r="E188" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="F188" s="89"/>
+      <c r="F188" s="105"/>
       <c r="G188" s="8" t="s">
         <v>319</v>
       </c>
@@ -13789,7 +13789,7 @@
       <c r="U188" s="8"/>
     </row>
     <row r="189" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A189" s="89"/>
+      <c r="A189" s="105"/>
       <c r="B189" s="6">
         <v>45539</v>
       </c>
@@ -13802,7 +13802,7 @@
       <c r="E189" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="F189" s="89"/>
+      <c r="F189" s="105"/>
       <c r="G189" s="8" t="s">
         <v>320</v>
       </c>
@@ -13842,7 +13842,7 @@
       <c r="U189" s="8"/>
     </row>
     <row r="190" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A190" s="89"/>
+      <c r="A190" s="105"/>
       <c r="B190" s="6">
         <v>45539</v>
       </c>
@@ -13855,7 +13855,7 @@
       <c r="E190" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="F190" s="89"/>
+      <c r="F190" s="105"/>
       <c r="G190" s="8" t="s">
         <v>321</v>
       </c>
@@ -13897,7 +13897,7 @@
       <c r="U190" s="8"/>
     </row>
     <row r="191" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A191" s="89"/>
+      <c r="A191" s="105"/>
       <c r="B191" s="6">
         <v>45539</v>
       </c>
@@ -13910,7 +13910,7 @@
       <c r="E191" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="F191" s="89"/>
+      <c r="F191" s="105"/>
       <c r="G191" s="8" t="s">
         <v>322</v>
       </c>
@@ -13950,7 +13950,7 @@
       <c r="U191" s="8"/>
     </row>
     <row r="192" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A192" s="89"/>
+      <c r="A192" s="105"/>
       <c r="B192" s="6">
         <v>45539</v>
       </c>
@@ -13963,7 +13963,7 @@
       <c r="E192" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="F192" s="89"/>
+      <c r="F192" s="105"/>
       <c r="G192" s="8" t="s">
         <v>323</v>
       </c>
@@ -14005,7 +14005,7 @@
       <c r="U192" s="8"/>
     </row>
     <row r="193" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A193" s="89"/>
+      <c r="A193" s="105"/>
       <c r="B193" s="6">
         <v>45539</v>
       </c>
@@ -14018,7 +14018,7 @@
       <c r="E193" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="F193" s="89"/>
+      <c r="F193" s="105"/>
       <c r="G193" s="8" t="s">
         <v>324</v>
       </c>
@@ -14058,7 +14058,7 @@
       <c r="U193" s="8"/>
     </row>
     <row r="194" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A194" s="96" t="s">
+      <c r="A194" s="106" t="s">
         <v>325</v>
       </c>
       <c r="B194" s="3">
@@ -14073,7 +14073,7 @@
       <c r="E194" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="F194" s="97" t="s">
+      <c r="F194" s="101" t="s">
         <v>330</v>
       </c>
       <c r="G194" s="2" t="s">
@@ -14117,7 +14117,7 @@
       <c r="U194" s="2"/>
     </row>
     <row r="195" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A195" s="96"/>
+      <c r="A195" s="106"/>
       <c r="B195" s="3">
         <v>45569</v>
       </c>
@@ -14130,7 +14130,7 @@
       <c r="E195" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="F195" s="98"/>
+      <c r="F195" s="102"/>
       <c r="G195" s="2" t="s">
         <v>332</v>
       </c>
@@ -14170,7 +14170,7 @@
       <c r="U195" s="2"/>
     </row>
     <row r="196" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A196" s="96"/>
+      <c r="A196" s="106"/>
       <c r="B196" s="3">
         <v>45569</v>
       </c>
@@ -14183,7 +14183,7 @@
       <c r="E196" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="F196" s="98"/>
+      <c r="F196" s="102"/>
       <c r="G196" s="2" t="s">
         <v>333</v>
       </c>
@@ -14225,7 +14225,7 @@
       <c r="U196" s="2"/>
     </row>
     <row r="197" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A197" s="96"/>
+      <c r="A197" s="106"/>
       <c r="B197" s="3">
         <v>45569</v>
       </c>
@@ -14238,7 +14238,7 @@
       <c r="E197" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="F197" s="98"/>
+      <c r="F197" s="102"/>
       <c r="G197" s="2" t="s">
         <v>334</v>
       </c>
@@ -14278,7 +14278,7 @@
       <c r="U197" s="2"/>
     </row>
     <row r="198" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A198" s="96"/>
+      <c r="A198" s="106"/>
       <c r="B198" s="3">
         <v>45569</v>
       </c>
@@ -14291,7 +14291,7 @@
       <c r="E198" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="F198" s="98"/>
+      <c r="F198" s="102"/>
       <c r="G198" s="2" t="s">
         <v>335</v>
       </c>
@@ -14333,7 +14333,7 @@
       <c r="U198" s="2"/>
     </row>
     <row r="199" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A199" s="96"/>
+      <c r="A199" s="106"/>
       <c r="B199" s="3">
         <v>45569</v>
       </c>
@@ -14346,7 +14346,7 @@
       <c r="E199" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="F199" s="98"/>
+      <c r="F199" s="102"/>
       <c r="G199" s="2" t="s">
         <v>336</v>
       </c>
@@ -14386,7 +14386,7 @@
       <c r="U199" s="2"/>
     </row>
     <row r="200" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A200" s="96"/>
+      <c r="A200" s="106"/>
       <c r="B200" s="3">
         <v>45569</v>
       </c>
@@ -14399,7 +14399,7 @@
       <c r="E200" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="F200" s="98"/>
+      <c r="F200" s="102"/>
       <c r="G200" s="2" t="s">
         <v>337</v>
       </c>
@@ -14441,7 +14441,7 @@
       <c r="U200" s="2"/>
     </row>
     <row r="201" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A201" s="96"/>
+      <c r="A201" s="106"/>
       <c r="B201" s="3">
         <v>45569</v>
       </c>
@@ -14454,7 +14454,7 @@
       <c r="E201" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="F201" s="99"/>
+      <c r="F201" s="103"/>
       <c r="G201" s="2" t="s">
         <v>338</v>
       </c>
@@ -14494,7 +14494,7 @@
       <c r="U201" s="2"/>
     </row>
     <row r="202" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A202" s="89" t="s">
+      <c r="A202" s="105" t="s">
         <v>339</v>
       </c>
       <c r="B202" s="6">
@@ -14509,7 +14509,7 @@
       <c r="E202" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="F202" s="90" t="s">
+      <c r="F202" s="92" t="s">
         <v>342</v>
       </c>
       <c r="G202" s="8" t="s">
@@ -14553,7 +14553,7 @@
       <c r="U202" s="8"/>
     </row>
     <row r="203" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A203" s="89"/>
+      <c r="A203" s="105"/>
       <c r="B203" s="6">
         <v>45570</v>
       </c>
@@ -14566,7 +14566,7 @@
       <c r="E203" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="F203" s="106"/>
+      <c r="F203" s="107"/>
       <c r="G203" s="8" t="s">
         <v>344</v>
       </c>
@@ -14606,7 +14606,7 @@
       <c r="U203" s="8"/>
     </row>
     <row r="204" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A204" s="89"/>
+      <c r="A204" s="105"/>
       <c r="B204" s="6">
         <v>45570</v>
       </c>
@@ -14619,7 +14619,7 @@
       <c r="E204" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="F204" s="106"/>
+      <c r="F204" s="107"/>
       <c r="G204" s="8" t="s">
         <v>345</v>
       </c>
@@ -14661,7 +14661,7 @@
       <c r="U204" s="8"/>
     </row>
     <row r="205" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A205" s="89"/>
+      <c r="A205" s="105"/>
       <c r="B205" s="6">
         <v>45570</v>
       </c>
@@ -14674,7 +14674,7 @@
       <c r="E205" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="F205" s="106"/>
+      <c r="F205" s="107"/>
       <c r="G205" s="8" t="s">
         <v>346</v>
       </c>
@@ -14714,7 +14714,7 @@
       <c r="U205" s="8"/>
     </row>
     <row r="206" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A206" s="89"/>
+      <c r="A206" s="105"/>
       <c r="B206" s="6">
         <v>45570</v>
       </c>
@@ -14727,7 +14727,7 @@
       <c r="E206" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="F206" s="106"/>
+      <c r="F206" s="107"/>
       <c r="G206" s="8" t="s">
         <v>347</v>
       </c>
@@ -14769,7 +14769,7 @@
       <c r="U206" s="8"/>
     </row>
     <row r="207" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A207" s="89"/>
+      <c r="A207" s="105"/>
       <c r="B207" s="6">
         <v>45570</v>
       </c>
@@ -14782,7 +14782,7 @@
       <c r="E207" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="F207" s="106"/>
+      <c r="F207" s="107"/>
       <c r="G207" s="8" t="s">
         <v>348</v>
       </c>
@@ -14822,7 +14822,7 @@
       <c r="U207" s="8"/>
     </row>
     <row r="208" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A208" s="89"/>
+      <c r="A208" s="105"/>
       <c r="B208" s="6">
         <v>45570</v>
       </c>
@@ -14835,7 +14835,7 @@
       <c r="E208" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="F208" s="106"/>
+      <c r="F208" s="107"/>
       <c r="G208" s="8" t="s">
         <v>349</v>
       </c>
@@ -14877,7 +14877,7 @@
       <c r="U208" s="8"/>
     </row>
     <row r="209" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A209" s="89"/>
+      <c r="A209" s="105"/>
       <c r="B209" s="6">
         <v>45570</v>
       </c>
@@ -14890,7 +14890,7 @@
       <c r="E209" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="F209" s="107"/>
+      <c r="F209" s="108"/>
       <c r="G209" s="8" t="s">
         <v>350</v>
       </c>
@@ -14930,7 +14930,7 @@
       <c r="U209" s="8"/>
     </row>
     <row r="210" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A210" s="96" t="s">
+      <c r="A210" s="106" t="s">
         <v>365</v>
       </c>
       <c r="B210" s="3">
@@ -14945,7 +14945,7 @@
       <c r="E210" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="F210" s="97" t="s">
+      <c r="F210" s="101" t="s">
         <v>355</v>
       </c>
       <c r="G210" s="2" t="s">
@@ -14989,7 +14989,7 @@
       <c r="U210" s="2"/>
     </row>
     <row r="211" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A211" s="96"/>
+      <c r="A211" s="106"/>
       <c r="B211" s="3">
         <v>45586</v>
       </c>
@@ -15002,7 +15002,7 @@
       <c r="E211" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="F211" s="98"/>
+      <c r="F211" s="102"/>
       <c r="G211" s="2" t="s">
         <v>357</v>
       </c>
@@ -15042,7 +15042,7 @@
       <c r="U211" s="2"/>
     </row>
     <row r="212" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A212" s="96"/>
+      <c r="A212" s="106"/>
       <c r="B212" s="3">
         <v>45586</v>
       </c>
@@ -15055,7 +15055,7 @@
       <c r="E212" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="F212" s="98"/>
+      <c r="F212" s="102"/>
       <c r="G212" s="2" t="s">
         <v>358</v>
       </c>
@@ -15097,7 +15097,7 @@
       <c r="U212" s="2"/>
     </row>
     <row r="213" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A213" s="96"/>
+      <c r="A213" s="106"/>
       <c r="B213" s="3">
         <v>45586</v>
       </c>
@@ -15110,7 +15110,7 @@
       <c r="E213" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="F213" s="98"/>
+      <c r="F213" s="102"/>
       <c r="G213" s="2" t="s">
         <v>359</v>
       </c>
@@ -15152,7 +15152,7 @@
       </c>
     </row>
     <row r="214" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A214" s="96"/>
+      <c r="A214" s="106"/>
       <c r="B214" s="3">
         <v>45586</v>
       </c>
@@ -15165,7 +15165,7 @@
       <c r="E214" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="F214" s="98"/>
+      <c r="F214" s="102"/>
       <c r="G214" s="2" t="s">
         <v>360</v>
       </c>
@@ -15207,7 +15207,7 @@
       <c r="U214" s="2"/>
     </row>
     <row r="215" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A215" s="96"/>
+      <c r="A215" s="106"/>
       <c r="B215" s="3">
         <v>45586</v>
       </c>
@@ -15220,7 +15220,7 @@
       <c r="E215" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="F215" s="98"/>
+      <c r="F215" s="102"/>
       <c r="G215" s="2" t="s">
         <v>361</v>
       </c>
@@ -15260,7 +15260,7 @@
       <c r="U215" s="2"/>
     </row>
     <row r="216" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A216" s="96"/>
+      <c r="A216" s="106"/>
       <c r="B216" s="3">
         <v>45586</v>
       </c>
@@ -15273,7 +15273,7 @@
       <c r="E216" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="F216" s="98"/>
+      <c r="F216" s="102"/>
       <c r="G216" s="2" t="s">
         <v>362</v>
       </c>
@@ -15315,7 +15315,7 @@
       <c r="U216" s="2"/>
     </row>
     <row r="217" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A217" s="96"/>
+      <c r="A217" s="106"/>
       <c r="B217" s="3">
         <v>45586</v>
       </c>
@@ -15328,7 +15328,7 @@
       <c r="E217" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="F217" s="99"/>
+      <c r="F217" s="103"/>
       <c r="G217" s="2" t="s">
         <v>363</v>
       </c>
@@ -15368,7 +15368,7 @@
       <c r="U217" s="2"/>
     </row>
     <row r="218" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A218" s="108" t="s">
+      <c r="A218" s="88" t="s">
         <v>366</v>
       </c>
       <c r="B218" s="40">
@@ -15383,7 +15383,7 @@
       <c r="E218" s="42" t="s">
         <v>369</v>
       </c>
-      <c r="F218" s="109" t="s">
+      <c r="F218" s="89" t="s">
         <v>371</v>
       </c>
       <c r="G218" s="44" t="s">
@@ -15421,7 +15421,7 @@
       </c>
     </row>
     <row r="219" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A219" s="108"/>
+      <c r="A219" s="88"/>
       <c r="B219" s="40">
         <v>45615</v>
       </c>
@@ -15434,7 +15434,7 @@
       <c r="E219" s="42" t="s">
         <v>369</v>
       </c>
-      <c r="F219" s="110"/>
+      <c r="F219" s="90"/>
       <c r="G219" s="42" t="s">
         <v>373</v>
       </c>
@@ -15480,7 +15480,7 @@
       </c>
     </row>
     <row r="220" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A220" s="108"/>
+      <c r="A220" s="88"/>
       <c r="B220" s="40">
         <v>45615</v>
       </c>
@@ -15493,7 +15493,7 @@
       <c r="E220" s="42" t="s">
         <v>369</v>
       </c>
-      <c r="F220" s="110"/>
+      <c r="F220" s="90"/>
       <c r="G220" s="42" t="s">
         <v>374</v>
       </c>
@@ -15539,7 +15539,7 @@
       </c>
     </row>
     <row r="221" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A221" s="108"/>
+      <c r="A221" s="88"/>
       <c r="B221" s="40">
         <v>45615</v>
       </c>
@@ -15552,7 +15552,7 @@
       <c r="E221" s="42" t="s">
         <v>369</v>
       </c>
-      <c r="F221" s="110"/>
+      <c r="F221" s="90"/>
       <c r="G221" s="44" t="s">
         <v>375</v>
       </c>
@@ -15588,7 +15588,7 @@
       </c>
     </row>
     <row r="222" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A222" s="108"/>
+      <c r="A222" s="88"/>
       <c r="B222" s="40">
         <v>45615</v>
       </c>
@@ -15601,7 +15601,7 @@
       <c r="E222" s="42" t="s">
         <v>370</v>
       </c>
-      <c r="F222" s="110"/>
+      <c r="F222" s="90"/>
       <c r="G222" s="42" t="s">
         <v>376</v>
       </c>
@@ -15643,7 +15643,7 @@
       <c r="U222" s="42"/>
     </row>
     <row r="223" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A223" s="108"/>
+      <c r="A223" s="88"/>
       <c r="B223" s="40">
         <v>45615</v>
       </c>
@@ -15656,7 +15656,7 @@
       <c r="E223" s="42" t="s">
         <v>370</v>
       </c>
-      <c r="F223" s="110"/>
+      <c r="F223" s="90"/>
       <c r="G223" s="42" t="s">
         <v>377</v>
       </c>
@@ -15696,7 +15696,7 @@
       <c r="U223" s="42"/>
     </row>
     <row r="224" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A224" s="108"/>
+      <c r="A224" s="88"/>
       <c r="B224" s="40">
         <v>45615</v>
       </c>
@@ -15709,7 +15709,7 @@
       <c r="E224" s="42" t="s">
         <v>370</v>
       </c>
-      <c r="F224" s="110"/>
+      <c r="F224" s="90"/>
       <c r="G224" s="42" t="s">
         <v>378</v>
       </c>
@@ -15754,8 +15754,8 @@
         <v>441</v>
       </c>
     </row>
-    <row r="225" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A225" s="108"/>
+    <row r="225" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A225" s="88"/>
       <c r="B225" s="40">
         <v>45615</v>
       </c>
@@ -15768,7 +15768,7 @@
       <c r="E225" s="42" t="s">
         <v>370</v>
       </c>
-      <c r="F225" s="111"/>
+      <c r="F225" s="91"/>
       <c r="G225" s="44" t="s">
         <v>379</v>
       </c>
@@ -15803,8 +15803,8 @@
         <v>440</v>
       </c>
     </row>
-    <row r="226" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A226" s="102" t="s">
+    <row r="226" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A226" s="111" t="s">
         <v>410</v>
       </c>
       <c r="B226" s="3">
@@ -15819,7 +15819,7 @@
       <c r="E226" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="F226" s="105" t="s">
+      <c r="F226" s="112" t="s">
         <v>411</v>
       </c>
       <c r="G226" s="2" t="s">
@@ -15866,8 +15866,8 @@
         <v>441</v>
       </c>
     </row>
-    <row r="227" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A227" s="103"/>
+    <row r="227" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A227" s="109"/>
       <c r="B227" s="3">
         <v>45714</v>
       </c>
@@ -15880,7 +15880,7 @@
       <c r="E227" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="F227" s="105"/>
+      <c r="F227" s="112"/>
       <c r="G227" s="44" t="s">
         <v>399</v>
       </c>
@@ -15915,8 +15915,8 @@
         <v>440</v>
       </c>
     </row>
-    <row r="228" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A228" s="103"/>
+    <row r="228" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A228" s="109"/>
       <c r="B228" s="3">
         <v>45714</v>
       </c>
@@ -15929,7 +15929,7 @@
       <c r="E228" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="F228" s="105"/>
+      <c r="F228" s="112"/>
       <c r="G228" s="2" t="s">
         <v>400</v>
       </c>
@@ -15974,8 +15974,8 @@
         <v>441</v>
       </c>
     </row>
-    <row r="229" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A229" s="103"/>
+    <row r="229" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A229" s="109"/>
       <c r="B229" s="3">
         <v>45714</v>
       </c>
@@ -15988,7 +15988,7 @@
       <c r="E229" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="F229" s="105"/>
+      <c r="F229" s="112"/>
       <c r="G229" s="44" t="s">
         <v>401</v>
       </c>
@@ -16023,8 +16023,8 @@
         <v>440</v>
       </c>
     </row>
-    <row r="230" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A230" s="103"/>
+    <row r="230" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A230" s="109"/>
       <c r="B230" s="3">
         <v>45714</v>
       </c>
@@ -16037,7 +16037,7 @@
       <c r="E230" s="38" t="s">
         <v>417</v>
       </c>
-      <c r="F230" s="105"/>
+      <c r="F230" s="112"/>
       <c r="G230" s="2" t="s">
         <v>402</v>
       </c>
@@ -16078,8 +16078,8 @@
       </c>
       <c r="U230" s="2"/>
     </row>
-    <row r="231" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A231" s="103"/>
+    <row r="231" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A231" s="109"/>
       <c r="B231" s="3">
         <v>45714</v>
       </c>
@@ -16092,7 +16092,7 @@
       <c r="E231" s="38" t="s">
         <v>417</v>
       </c>
-      <c r="F231" s="105"/>
+      <c r="F231" s="112"/>
       <c r="G231" s="2" t="s">
         <v>403</v>
       </c>
@@ -16127,8 +16127,8 @@
       <c r="T231" s="2"/>
       <c r="U231" s="2"/>
     </row>
-    <row r="232" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A232" s="103"/>
+    <row r="232" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A232" s="109"/>
       <c r="B232" s="3">
         <v>45714</v>
       </c>
@@ -16141,7 +16141,7 @@
       <c r="E232" s="38" t="s">
         <v>419</v>
       </c>
-      <c r="F232" s="105"/>
+      <c r="F232" s="112"/>
       <c r="G232" s="44" t="s">
         <v>404</v>
       </c>
@@ -16176,8 +16176,8 @@
         <v>440</v>
       </c>
     </row>
-    <row r="233" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A233" s="103"/>
+    <row r="233" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A233" s="109"/>
       <c r="B233" s="3">
         <v>45714</v>
       </c>
@@ -16190,7 +16190,7 @@
       <c r="E233" s="38" t="s">
         <v>419</v>
       </c>
-      <c r="F233" s="105"/>
+      <c r="F233" s="112"/>
       <c r="G233" s="44" t="s">
         <v>405</v>
       </c>
@@ -16225,8 +16225,8 @@
         <v>440</v>
       </c>
     </row>
-    <row r="234" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A234" s="103"/>
+    <row r="234" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A234" s="109"/>
       <c r="B234" s="3">
         <v>45714</v>
       </c>
@@ -16239,7 +16239,7 @@
       <c r="E234" s="38" t="s">
         <v>421</v>
       </c>
-      <c r="F234" s="105"/>
+      <c r="F234" s="112"/>
       <c r="G234" s="2" t="s">
         <v>406</v>
       </c>
@@ -16284,8 +16284,8 @@
         <v>441</v>
       </c>
     </row>
-    <row r="235" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A235" s="103"/>
+    <row r="235" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A235" s="109"/>
       <c r="B235" s="3">
         <v>45714</v>
       </c>
@@ -16298,7 +16298,7 @@
       <c r="E235" s="38" t="s">
         <v>421</v>
       </c>
-      <c r="F235" s="105"/>
+      <c r="F235" s="112"/>
       <c r="G235" s="44" t="s">
         <v>407</v>
       </c>
@@ -16333,8 +16333,8 @@
         <v>440</v>
       </c>
     </row>
-    <row r="236" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A236" s="103"/>
+    <row r="236" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A236" s="109"/>
       <c r="B236" s="3">
         <v>45714</v>
       </c>
@@ -16347,7 +16347,7 @@
       <c r="E236" s="38" t="s">
         <v>423</v>
       </c>
-      <c r="F236" s="105"/>
+      <c r="F236" s="112"/>
       <c r="G236" s="2" t="s">
         <v>408</v>
       </c>
@@ -16392,8 +16392,8 @@
         <v>442</v>
       </c>
     </row>
-    <row r="237" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A237" s="104"/>
+    <row r="237" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A237" s="110"/>
       <c r="B237" s="3">
         <v>45714</v>
       </c>
@@ -16406,7 +16406,7 @@
       <c r="E237" s="38" t="s">
         <v>423</v>
       </c>
-      <c r="F237" s="105"/>
+      <c r="F237" s="112"/>
       <c r="G237" s="44" t="s">
         <v>409</v>
       </c>
@@ -16441,8 +16441,8 @@
         <v>440</v>
       </c>
     </row>
-    <row r="238" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A238" s="89" t="s">
+    <row r="238" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A238" s="105" t="s">
         <v>433</v>
       </c>
       <c r="B238" s="6">
@@ -16457,7 +16457,7 @@
       <c r="E238" s="8" t="s">
         <v>435</v>
       </c>
-      <c r="F238" s="88" t="s">
+      <c r="F238" s="104" t="s">
         <v>432</v>
       </c>
       <c r="G238" s="8" t="s">
@@ -16496,12 +16496,10 @@
       <c r="T238" s="20" t="s">
         <v>381</v>
       </c>
-      <c r="U238" s="8">
-        <v>7.7270086131315026</v>
-      </c>
-    </row>
-    <row r="239" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A239" s="89"/>
+      <c r="U238" s="8"/>
+    </row>
+    <row r="239" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A239" s="105"/>
       <c r="B239" s="6">
         <v>45744</v>
       </c>
@@ -16514,7 +16512,7 @@
       <c r="E239" s="8" t="s">
         <v>435</v>
       </c>
-      <c r="F239" s="88"/>
+      <c r="F239" s="104"/>
       <c r="G239" s="8" t="s">
         <v>425</v>
       </c>
@@ -16548,12 +16546,9 @@
       <c r="S239" s="8"/>
       <c r="T239" s="8"/>
       <c r="U239" s="8"/>
-      <c r="V239">
-        <v>1.1655575505652216E-2</v>
-      </c>
-    </row>
-    <row r="240" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A240" s="89"/>
+    </row>
+    <row r="240" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A240" s="105"/>
       <c r="B240" s="6">
         <v>45744</v>
       </c>
@@ -16566,7 +16561,7 @@
       <c r="E240" s="8" t="s">
         <v>435</v>
       </c>
-      <c r="F240" s="88"/>
+      <c r="F240" s="104"/>
       <c r="G240" s="8" t="s">
         <v>426</v>
       </c>
@@ -16599,12 +16594,10 @@
         <v>2059.2738181639183</v>
       </c>
       <c r="T240" s="8"/>
-      <c r="U240" s="8">
-        <v>7.7300002099625784</v>
-      </c>
-    </row>
-    <row r="241" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A241" s="89"/>
+      <c r="U240" s="8"/>
+    </row>
+    <row r="241" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A241" s="105"/>
       <c r="B241" s="6">
         <v>45744</v>
       </c>
@@ -16617,7 +16610,7 @@
       <c r="E241" s="8" t="s">
         <v>435</v>
       </c>
-      <c r="F241" s="88"/>
+      <c r="F241" s="104"/>
       <c r="G241" s="8" t="s">
         <v>427</v>
       </c>
@@ -16651,12 +16644,9 @@
       <c r="S241" s="8"/>
       <c r="T241" s="8"/>
       <c r="U241" s="8"/>
-      <c r="V241">
-        <v>1.167945701061246E-2</v>
-      </c>
-    </row>
-    <row r="242" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A242" s="89"/>
+    </row>
+    <row r="242" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A242" s="105"/>
       <c r="B242" s="6">
         <v>45744</v>
       </c>
@@ -16669,7 +16659,7 @@
       <c r="E242" s="8" t="s">
         <v>437</v>
       </c>
-      <c r="F242" s="88"/>
+      <c r="F242" s="104"/>
       <c r="G242" s="8" t="s">
         <v>428</v>
       </c>
@@ -16702,12 +16692,10 @@
         <v>2067.8083389613585</v>
       </c>
       <c r="T242" s="8"/>
-      <c r="U242" s="8">
-        <v>7.7374167736160659</v>
-      </c>
-    </row>
-    <row r="243" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A243" s="89"/>
+      <c r="U242" s="8"/>
+    </row>
+    <row r="243" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A243" s="105"/>
       <c r="B243" s="6">
         <v>45744</v>
       </c>
@@ -16720,7 +16708,7 @@
       <c r="E243" s="8" t="s">
         <v>437</v>
       </c>
-      <c r="F243" s="88"/>
+      <c r="F243" s="104"/>
       <c r="G243" s="8" t="s">
         <v>429</v>
       </c>
@@ -16754,12 +16742,9 @@
       <c r="S243" s="8"/>
       <c r="T243" s="8"/>
       <c r="U243" s="8"/>
-      <c r="V243">
-        <v>4.7575216732358427E-3</v>
-      </c>
-    </row>
-    <row r="244" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A244" s="89"/>
+    </row>
+    <row r="244" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A244" s="105"/>
       <c r="B244" s="6">
         <v>45744</v>
       </c>
@@ -16772,7 +16757,7 @@
       <c r="E244" s="8" t="s">
         <v>439</v>
       </c>
-      <c r="F244" s="88"/>
+      <c r="F244" s="104"/>
       <c r="G244" s="8" t="s">
         <v>430</v>
       </c>
@@ -16805,12 +16790,10 @@
         <v>2068.2022399212406</v>
       </c>
       <c r="T244" s="8"/>
-      <c r="U244" s="8">
-        <v>7.7385272185687368</v>
-      </c>
-    </row>
-    <row r="245" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A245" s="89"/>
+      <c r="U244" s="8"/>
+    </row>
+    <row r="245" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A245" s="105"/>
       <c r="B245" s="6">
         <v>45744</v>
       </c>
@@ -16823,7 +16806,7 @@
       <c r="E245" s="8" t="s">
         <v>439</v>
       </c>
-      <c r="F245" s="88"/>
+      <c r="F245" s="104"/>
       <c r="G245" s="8" t="s">
         <v>431</v>
       </c>
@@ -16857,57 +16840,31 @@
       <c r="S245" s="8"/>
       <c r="T245" s="8"/>
       <c r="U245" s="8"/>
-      <c r="V245">
-        <v>6.8032015887755648E-3</v>
-      </c>
-    </row>
-    <row r="248" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="Q248" s="8">
-        <v>2183.5494409558341</v>
-      </c>
-      <c r="R248" s="8">
-        <v>2059.2738181639183</v>
-      </c>
-      <c r="S248" s="8">
-        <v>7.7416796669731909</v>
-      </c>
-    </row>
-    <row r="249" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="Q249" s="8">
-        <v>2195.5575788585634</v>
-      </c>
-      <c r="R249" s="8">
-        <v>2067.8083389613585</v>
-      </c>
-      <c r="S249" s="8">
-        <v>7.7421742952893018</v>
-      </c>
-    </row>
-    <row r="250" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="Q250" s="8">
-        <v>2196.4039235697837</v>
-      </c>
-      <c r="R250" s="8">
-        <v>2068.2022399212406</v>
-      </c>
-      <c r="S250" s="8">
-        <v>7.7453304201575124</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="A218:A225"/>
-    <mergeCell ref="F218:F225"/>
-    <mergeCell ref="A138:A149"/>
-    <mergeCell ref="F138:F149"/>
-    <mergeCell ref="A150:A161"/>
-    <mergeCell ref="F150:F161"/>
-    <mergeCell ref="A182:A193"/>
-    <mergeCell ref="F182:F193"/>
-    <mergeCell ref="A210:A217"/>
-    <mergeCell ref="F210:F217"/>
-    <mergeCell ref="A202:A209"/>
-    <mergeCell ref="F202:F209"/>
+    <mergeCell ref="F238:F245"/>
+    <mergeCell ref="A238:A245"/>
+    <mergeCell ref="A114:A125"/>
+    <mergeCell ref="F114:F125"/>
+    <mergeCell ref="A102:A113"/>
+    <mergeCell ref="F102:F113"/>
+    <mergeCell ref="A194:A201"/>
+    <mergeCell ref="F194:F201"/>
+    <mergeCell ref="A126:A137"/>
+    <mergeCell ref="F126:F137"/>
+    <mergeCell ref="A162:A169"/>
+    <mergeCell ref="F162:F169"/>
+    <mergeCell ref="A170:A181"/>
+    <mergeCell ref="F170:F181"/>
+    <mergeCell ref="A226:A237"/>
+    <mergeCell ref="F226:F237"/>
+    <mergeCell ref="A58:A65"/>
+    <mergeCell ref="F58:F65"/>
+    <mergeCell ref="A66:A73"/>
+    <mergeCell ref="F66:F73"/>
+    <mergeCell ref="A74:A77"/>
+    <mergeCell ref="F74:F77"/>
     <mergeCell ref="A94:A101"/>
     <mergeCell ref="F94:F101"/>
     <mergeCell ref="A2:A13"/>
@@ -16924,28 +16881,18 @@
     <mergeCell ref="A46:A57"/>
     <mergeCell ref="F38:F45"/>
     <mergeCell ref="F46:F57"/>
-    <mergeCell ref="A58:A65"/>
-    <mergeCell ref="F58:F65"/>
-    <mergeCell ref="A66:A73"/>
-    <mergeCell ref="F66:F73"/>
-    <mergeCell ref="A74:A77"/>
-    <mergeCell ref="F74:F77"/>
-    <mergeCell ref="F238:F245"/>
-    <mergeCell ref="A238:A245"/>
-    <mergeCell ref="A114:A125"/>
-    <mergeCell ref="F114:F125"/>
-    <mergeCell ref="A102:A113"/>
-    <mergeCell ref="F102:F113"/>
-    <mergeCell ref="A194:A201"/>
-    <mergeCell ref="F194:F201"/>
-    <mergeCell ref="A126:A137"/>
-    <mergeCell ref="F126:F137"/>
-    <mergeCell ref="A162:A169"/>
-    <mergeCell ref="F162:F169"/>
-    <mergeCell ref="A170:A181"/>
-    <mergeCell ref="F170:F181"/>
-    <mergeCell ref="A226:A237"/>
-    <mergeCell ref="F226:F237"/>
+    <mergeCell ref="A218:A225"/>
+    <mergeCell ref="F218:F225"/>
+    <mergeCell ref="A138:A149"/>
+    <mergeCell ref="F138:F149"/>
+    <mergeCell ref="A150:A161"/>
+    <mergeCell ref="F150:F161"/>
+    <mergeCell ref="A182:A193"/>
+    <mergeCell ref="F182:F193"/>
+    <mergeCell ref="A210:A217"/>
+    <mergeCell ref="F210:F217"/>
+    <mergeCell ref="A202:A209"/>
+    <mergeCell ref="F202:F209"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16958,8 +16905,8 @@
   <dimension ref="A1:W232"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A212" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K237" sqref="K237"/>
+      <pane ySplit="1" topLeftCell="A218" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L248" sqref="L248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>